<commit_message>
rename generations cols in Butterfly matrix, add Poaceae column to forage_plant_locations spreadsheet
</commit_message>
<xml_diff>
--- a/Butterfly matrix.xlsx
+++ b/Butterfly matrix.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64431EEC-755E-F94C-B6BB-D62C920AD717}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D677BD54-8B7B-E743-A4F2-D1F92AE7A1D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Species Set" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="2" r:id="rId2"/>
+    <sheet name="larvae forage plants" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -142,17 +143,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
   <si>
     <t>Species</t>
   </si>
   <si>
-    <t>Adult reliance</t>
-  </si>
-  <si>
-    <t>Larval reliance</t>
-  </si>
-  <si>
     <t>Ad_H_hab</t>
   </si>
   <si>
@@ -288,21 +283,6 @@
     <t>L_R_late</t>
   </si>
   <si>
-    <t>L_H_damp plant</t>
-  </si>
-  <si>
-    <t>L_M_damp plant</t>
-  </si>
-  <si>
-    <t>L_CA_damp plant</t>
-  </si>
-  <si>
-    <t>L_CG_damp plant</t>
-  </si>
-  <si>
-    <t>L_R_damp plant</t>
-  </si>
-  <si>
     <t>Adult forage plant* hab comps</t>
   </si>
   <si>
@@ -492,20 +472,53 @@
     <t>LARVAE</t>
   </si>
   <si>
-    <t>Larval generations</t>
-  </si>
-  <si>
-    <t>1 (2 according to supp?)</t>
-  </si>
-  <si>
-    <t>Adult generations</t>
+    <t>Ad_generations</t>
+  </si>
+  <si>
+    <t>L_generations</t>
+  </si>
+  <si>
+    <t>Ad_reliance</t>
+  </si>
+  <si>
+    <t>L_reliance</t>
+  </si>
+  <si>
+    <t>Ad_H_damp</t>
+  </si>
+  <si>
+    <t>Ad_M_damp</t>
+  </si>
+  <si>
+    <t>Ad_CA_damp</t>
+  </si>
+  <si>
+    <t>Ad_CG_damp</t>
+  </si>
+  <si>
+    <t>Ad_R_damp</t>
+  </si>
+  <si>
+    <t>L_H_damp</t>
+  </si>
+  <si>
+    <t>L_M_damp</t>
+  </si>
+  <si>
+    <t>L_CA_damp</t>
+  </si>
+  <si>
+    <t>L_CG_damp</t>
+  </si>
+  <si>
+    <t>L_R_damp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,12 +538,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -715,29 +722,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -751,15 +740,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -771,6 +751,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1159,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AG19" sqref="AG19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1189,244 +1196,246 @@
     <col min="33" max="33" width="9.83203125" customWidth="1"/>
     <col min="42" max="42" width="9.83203125" customWidth="1"/>
     <col min="45" max="45" width="10.33203125" customWidth="1"/>
-    <col min="53" max="53" width="9.5" customWidth="1"/>
+    <col min="52" max="52" width="10.5" customWidth="1"/>
+    <col min="53" max="53" width="10.1640625" customWidth="1"/>
+    <col min="54" max="54" width="11" customWidth="1"/>
     <col min="55" max="55" width="10.1640625" customWidth="1"/>
     <col min="57" max="57" width="17.6640625" customWidth="1"/>
     <col min="58" max="58" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33"/>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
-      <c r="AS1" s="33"/>
-      <c r="AT1" s="33"/>
-      <c r="AU1" s="33"/>
-      <c r="AV1" s="33"/>
-      <c r="AW1" s="33"/>
-      <c r="AX1" s="33"/>
-      <c r="AY1" s="33"/>
-      <c r="AZ1" s="33"/>
-      <c r="BA1" s="33"/>
-      <c r="BB1" s="33"/>
-      <c r="BC1" s="33"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36"/>
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="36"/>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="36"/>
+      <c r="AV1" s="36"/>
+      <c r="AW1" s="36"/>
+      <c r="AX1" s="36"/>
+      <c r="AY1" s="36"/>
+      <c r="AZ1" s="36"/>
+      <c r="BA1" s="36"/>
+      <c r="BB1" s="36"/>
+      <c r="BC1" s="36"/>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.2">
-      <c r="F2" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-      <c r="AJ2" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="20"/>
-      <c r="AY2" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="25"/>
-      <c r="BB2" s="25"/>
-      <c r="BC2" s="25"/>
+      <c r="F2" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="38"/>
+      <c r="AV2" s="38"/>
+      <c r="AW2" s="38"/>
+      <c r="AX2" s="38"/>
+      <c r="AY2" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.2">
       <c r="F3" s="14" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA3" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB3" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC3" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD3" s="27" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA3" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB3" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC3" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD3" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="AE3" s="14" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="AF3" s="16" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="AG3" s="14" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="AH3" s="16" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="AI3" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ3" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="AN3" s="23"/>
-      <c r="AO3" s="23"/>
-      <c r="AP3" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="AQ3" s="21"/>
-      <c r="AR3" s="21"/>
-      <c r="AS3" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="AT3" s="23"/>
-      <c r="AU3" s="23"/>
-      <c r="AV3" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW3" s="21"/>
-      <c r="AX3" s="21"/>
-      <c r="AY3" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="AZ3" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="BA3" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="BB3" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="BC3" s="27" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="AJ3" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK3" s="30"/>
+      <c r="AL3" s="30"/>
+      <c r="AM3" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN3" s="31"/>
+      <c r="AO3" s="31"/>
+      <c r="AP3" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ3" s="30"/>
+      <c r="AR3" s="30"/>
+      <c r="AS3" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT3" s="31"/>
+      <c r="AU3" s="31"/>
+      <c r="AV3" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW3" s="30"/>
+      <c r="AX3" s="30"/>
+      <c r="AY3" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AZ3" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="BA3" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="BB3" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC3" s="21" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:58" ht="32" x14ac:dyDescent="0.2">
@@ -1434,178 +1443,178 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="W4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="X4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z4" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA4" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB4" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC4" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD4" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE4" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF4" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH4" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI4" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK4" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL4" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR4" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW4" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX4" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY4" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="S4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="T4" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="U4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="W4" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="X4" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y4" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z4" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA4" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB4" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC4" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD4" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE4" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG4" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH4" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI4" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ4" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK4" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL4" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM4" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN4" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO4" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP4" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ4" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR4" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS4" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT4" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU4" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV4" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW4" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="AX4" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="AY4" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="AZ4" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA4" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="BB4" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="BC4" s="28" t="s">
-        <v>52</v>
+      <c r="AZ4" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="BA4" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB4" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC4" s="22" t="s">
+        <v>122</v>
       </c>
       <c r="BD4" s="5"/>
       <c r="BE4" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="BF4" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B5" s="7">
         <v>3</v>
@@ -1614,7 +1623,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1779,7 +1788,7 @@
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -1953,7 +1962,7 @@
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B7" s="7">
         <v>3</v>
@@ -2127,7 +2136,7 @@
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B8" s="7">
         <v>3</v>
@@ -2301,7 +2310,7 @@
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B9" s="7">
         <v>2</v>
@@ -2475,7 +2484,7 @@
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7">
         <v>2</v>
@@ -2649,7 +2658,7 @@
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B11" s="7">
         <v>2</v>
@@ -2823,7 +2832,7 @@
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B12" s="7">
         <v>2</v>
@@ -2997,7 +3006,7 @@
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B13" s="7">
         <v>2</v>
@@ -3171,7 +3180,7 @@
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B14" s="7">
         <v>3</v>
@@ -3345,7 +3354,7 @@
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B15" s="7">
         <v>2</v>
@@ -3519,7 +3528,7 @@
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B16" s="7">
         <v>2</v>
@@ -3530,8 +3539,8 @@
       <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>117</v>
+      <c r="E16" s="7">
+        <v>2</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>
@@ -3693,7 +3702,7 @@
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B17" s="7">
         <v>2</v>
@@ -3867,7 +3876,7 @@
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B18" s="7">
         <v>3</v>
@@ -4041,7 +4050,7 @@
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B19" s="7">
         <v>3</v>
@@ -4215,7 +4224,7 @@
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B20" s="7">
         <v>1</v>
@@ -4389,7 +4398,7 @@
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B21" s="7">
         <v>2</v>
@@ -4563,7 +4572,7 @@
     </row>
     <row r="22" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B22" s="7">
         <v>2</v>
@@ -4737,7 +4746,7 @@
     </row>
     <row r="23" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B23" s="7">
         <v>2</v>
@@ -4911,7 +4920,7 @@
     </row>
     <row r="24" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B24" s="7">
         <v>3</v>
@@ -5085,7 +5094,7 @@
     </row>
     <row r="25" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B25" s="7">
         <v>3</v>
@@ -5259,7 +5268,7 @@
     </row>
     <row r="26" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B26" s="7">
         <v>2</v>
@@ -5433,7 +5442,7 @@
     </row>
     <row r="27" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B27" s="7">
         <v>2</v>
@@ -5607,7 +5616,7 @@
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B28" s="7">
         <v>1</v>
@@ -5787,13 +5796,13 @@
     <mergeCell ref="AE1:BC1"/>
     <mergeCell ref="AE2:AI2"/>
     <mergeCell ref="AJ2:AX2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:Y2"/>
     <mergeCell ref="AJ3:AL3"/>
     <mergeCell ref="AM3:AO3"/>
     <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="AS3:AU3"/>
     <mergeCell ref="AV3:AX3"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:Y2"/>
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="Q3:S3"/>
@@ -5821,210 +5830,353 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15139ED6-08F6-7542-82E2-485189D230BA}">
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added larval plant species to butterfly matrix
</commit_message>
<xml_diff>
--- a/Butterfly matrix.xlsx
+++ b/Butterfly matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D677BD54-8B7B-E743-A4F2-D1F92AE7A1D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBF1040-CAE7-154E-8A8D-B24BE49476D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <author>tc={474050C6-30EB-3142-8B55-53BB5FF6866F}</author>
   </authors>
   <commentList>
-    <comment ref="BE4" authorId="0" shapeId="0" xr:uid="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
+    <comment ref="CI4" authorId="0" shapeId="0" xr:uid="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
     This is Fa</t>
       </text>
     </comment>
-    <comment ref="BF4" authorId="1" shapeId="0" xr:uid="{100F15A9-7741-456F-AB72-27BB7A9AB780}">
+    <comment ref="CJ4" authorId="1" shapeId="0" xr:uid="{100F15A9-7741-456F-AB72-27BB7A9AB780}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="154">
   <si>
     <t>Species</t>
   </si>
@@ -512,13 +512,106 @@
   </si>
   <si>
     <t>L_R_damp</t>
+  </si>
+  <si>
+    <t>Aquifoliaceae</t>
+  </si>
+  <si>
+    <t>Araliaceae</t>
+  </si>
+  <si>
+    <t>Balsaminaceae</t>
+  </si>
+  <si>
+    <t>Boraginaceae</t>
+  </si>
+  <si>
+    <t>Campanulaceae</t>
+  </si>
+  <si>
+    <t>Cannabaceae</t>
+  </si>
+  <si>
+    <t>Caryophyllaceae</t>
+  </si>
+  <si>
+    <t>Compositae</t>
+  </si>
+  <si>
+    <t>Convolvulaceae</t>
+  </si>
+  <si>
+    <t>Cornaceae</t>
+  </si>
+  <si>
+    <t>Cruciferae</t>
+  </si>
+  <si>
+    <t>Dipsacaceae</t>
+  </si>
+  <si>
+    <t>Fabaceae</t>
+  </si>
+  <si>
+    <t>Grossulariaceae</t>
+  </si>
+  <si>
+    <t>Lamiaceae</t>
+  </si>
+  <si>
+    <t>Liliaceae</t>
+  </si>
+  <si>
+    <t>Lythraceae</t>
+  </si>
+  <si>
+    <t>Malvaceae</t>
+  </si>
+  <si>
+    <t>Onagraceae</t>
+  </si>
+  <si>
+    <t>Papaveraceae</t>
+  </si>
+  <si>
+    <t>Poaceae</t>
+  </si>
+  <si>
+    <t>Polygonaceae</t>
+  </si>
+  <si>
+    <t>Ranunculaceae</t>
+  </si>
+  <si>
+    <t>Rhamnaceae</t>
+  </si>
+  <si>
+    <t>Rosaceae</t>
+  </si>
+  <si>
+    <t>Salicaceae</t>
+  </si>
+  <si>
+    <t>Scrophulariaceae</t>
+  </si>
+  <si>
+    <t>Ulmaceae</t>
+  </si>
+  <si>
+    <t>Umbelliferae</t>
+  </si>
+  <si>
+    <t>Violaceae</t>
+  </si>
+  <si>
+    <t>Celastraceae</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +628,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -670,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -778,6 +877,16 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1123,10 +1232,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="BE4" dT="2020-01-20T13:33:41.57" personId="{DC903E8D-CC64-4CAD-9C70-13197F8FDC74}" id="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
+  <threadedComment ref="CI4" dT="2020-01-20T13:33:41.57" personId="{DC903E8D-CC64-4CAD-9C70-13197F8FDC74}" id="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
     <text>This is Fa</text>
   </threadedComment>
-  <threadedComment ref="BF4" dT="2020-01-20T13:33:54.11" personId="{DC903E8D-CC64-4CAD-9C70-13197F8FDC74}" id="{100F15A9-7741-456F-AB72-27BB7A9AB780}">
+  <threadedComment ref="CJ4" dT="2020-01-20T13:33:54.11" personId="{DC903E8D-CC64-4CAD-9C70-13197F8FDC74}" id="{100F15A9-7741-456F-AB72-27BB7A9AB780}">
     <text>This is Fl</text>
   </threadedComment>
   <threadedComment ref="E8" dT="2021-04-15T18:05:37.40" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{C66782A8-B31B-4B41-ABAC-0834AB6DC62E}">
@@ -1164,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF28"/>
+  <dimension ref="A1:CJ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AG19" sqref="AG19"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="AW6" sqref="AW6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1200,11 +1309,11 @@
     <col min="53" max="53" width="10.1640625" customWidth="1"/>
     <col min="54" max="54" width="11" customWidth="1"/>
     <col min="55" max="55" width="10.1640625" customWidth="1"/>
-    <col min="57" max="57" width="17.6640625" customWidth="1"/>
-    <col min="58" max="58" width="19.6640625" customWidth="1"/>
+    <col min="87" max="87" width="17.6640625" customWidth="1"/>
+    <col min="88" max="88" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.2">
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
       <c r="F1" s="34" t="s">
@@ -1261,8 +1370,39 @@
       <c r="BA1" s="36"/>
       <c r="BB1" s="36"/>
       <c r="BC1" s="36"/>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BD1" s="42"/>
+      <c r="BE1" s="42"/>
+      <c r="BF1" s="42"/>
+      <c r="BG1" s="42"/>
+      <c r="BH1" s="42"/>
+      <c r="BI1" s="42"/>
+      <c r="BJ1" s="42"/>
+      <c r="BK1" s="42"/>
+      <c r="BL1" s="42"/>
+      <c r="BM1" s="42"/>
+      <c r="BN1" s="42"/>
+      <c r="BO1" s="42"/>
+      <c r="BP1" s="42"/>
+      <c r="BQ1" s="42"/>
+      <c r="BR1" s="42"/>
+      <c r="BS1" s="42"/>
+      <c r="BT1" s="42"/>
+      <c r="BU1" s="42"/>
+      <c r="BV1" s="42"/>
+      <c r="BW1" s="42"/>
+      <c r="BX1" s="42"/>
+      <c r="BY1" s="42"/>
+      <c r="BZ1" s="42"/>
+      <c r="CA1" s="42"/>
+      <c r="CB1" s="42"/>
+      <c r="CC1" s="42"/>
+      <c r="CD1" s="42"/>
+      <c r="CE1" s="42"/>
+      <c r="CF1" s="42"/>
+      <c r="CG1" s="42"/>
+      <c r="CH1" s="42"/>
+    </row>
+    <row r="2" spans="1:88" x14ac:dyDescent="0.2">
       <c r="F2" s="37" t="s">
         <v>104</v>
       </c>
@@ -1326,7 +1466,7 @@
       <c r="BB2" s="32"/>
       <c r="BC2" s="32"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.2">
       <c r="F3" s="14" t="s">
         <v>99</v>
       </c>
@@ -1438,7 +1578,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:58" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:88" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1604,15 +1744,107 @@
       <c r="BC4" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="BD4" s="5"/>
-      <c r="BE4" s="6" t="s">
+      <c r="BD4" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="BE4" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="BF4" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="BG4" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="BH4" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="BI4" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="BJ4" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="BK4" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="BL4" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="BM4" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="BN4" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="BO4" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="BP4" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="BQ4" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="BR4" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS4" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="BT4" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="BU4" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="BV4" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="BW4" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="BX4" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="BY4" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="BZ4" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="CA4" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="CB4" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="CC4" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="CD4" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="CE4" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="CF4" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="CG4" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="CH4" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="CI4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="BF4" s="5" t="s">
+      <c r="CJ4" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>48</v>
       </c>
@@ -1778,15 +2010,19 @@
       <c r="BC5" s="7">
         <v>0</v>
       </c>
-      <c r="BD5" s="7"/>
-      <c r="BE5" s="12">
+      <c r="BE5" s="39"/>
+      <c r="BF5" s="39"/>
+      <c r="CB5">
+        <v>1</v>
+      </c>
+      <c r="CI5" s="12">
         <v>73</v>
       </c>
-      <c r="BF5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="CJ5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -1952,15 +2188,20 @@
       <c r="BC6" s="7">
         <v>0</v>
       </c>
-      <c r="BD6" s="7"/>
-      <c r="BE6" s="13">
+      <c r="BE6" s="40"/>
+      <c r="BF6" s="40"/>
+      <c r="CB6" s="41"/>
+      <c r="CC6">
+        <v>1</v>
+      </c>
+      <c r="CI6" s="13">
         <v>27</v>
       </c>
-      <c r="BF6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="CJ6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>50</v>
       </c>
@@ -2127,14 +2368,26 @@
         <v>0</v>
       </c>
       <c r="BD7" s="7"/>
-      <c r="BE7" s="12">
+      <c r="BI7">
+        <v>1</v>
+      </c>
+      <c r="BR7">
+        <v>1</v>
+      </c>
+      <c r="CD7">
+        <v>1</v>
+      </c>
+      <c r="CF7">
+        <v>1</v>
+      </c>
+      <c r="CI7" s="12">
         <v>73</v>
       </c>
-      <c r="BF7" s="7">
+      <c r="CJ7" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>51</v>
       </c>
@@ -2301,14 +2554,17 @@
         <v>0</v>
       </c>
       <c r="BD8" s="7"/>
-      <c r="BE8" s="12">
+      <c r="BQ8">
+        <v>1</v>
+      </c>
+      <c r="CI8" s="12">
         <v>59</v>
       </c>
-      <c r="BF8" s="1">
+      <c r="CJ8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>52</v>
       </c>
@@ -2475,14 +2731,18 @@
         <v>0</v>
       </c>
       <c r="BD9" s="7"/>
-      <c r="BE9" s="12">
+      <c r="BJ9" s="39"/>
+      <c r="BY9">
+        <v>1</v>
+      </c>
+      <c r="CI9" s="12">
         <v>29</v>
       </c>
-      <c r="BF9" s="1">
+      <c r="CJ9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>53</v>
       </c>
@@ -2649,14 +2909,17 @@
         <v>0</v>
       </c>
       <c r="BD10" s="7"/>
-      <c r="BE10" s="12">
+      <c r="BY10">
+        <v>1</v>
+      </c>
+      <c r="CI10" s="12">
         <v>41</v>
       </c>
-      <c r="BF10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="CJ10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -2823,14 +3086,17 @@
         <v>0</v>
       </c>
       <c r="BD11" s="7"/>
-      <c r="BE11" s="12">
+      <c r="BO11">
+        <v>1</v>
+      </c>
+      <c r="CI11" s="12">
         <v>73</v>
       </c>
-      <c r="BF11" s="1">
+      <c r="CJ11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
@@ -2996,15 +3262,35 @@
       <c r="BC12" s="7">
         <v>0</v>
       </c>
-      <c r="BD12" s="7"/>
-      <c r="BE12" s="12">
+      <c r="BD12" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE12" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK12">
+        <v>1</v>
+      </c>
+      <c r="BN12">
+        <v>1</v>
+      </c>
+      <c r="BQ12">
+        <v>1</v>
+      </c>
+      <c r="CB12">
+        <v>1</v>
+      </c>
+      <c r="CC12">
+        <v>1</v>
+      </c>
+      <c r="CI12" s="12">
         <v>59</v>
       </c>
-      <c r="BF12" s="1">
+      <c r="CJ12" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
@@ -3171,14 +3457,17 @@
         <v>0</v>
       </c>
       <c r="BD13" s="7"/>
-      <c r="BE13" s="12">
+      <c r="BY13">
+        <v>1</v>
+      </c>
+      <c r="CI13" s="12">
         <v>29</v>
       </c>
-      <c r="BF13" s="1">
+      <c r="CJ13" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>57</v>
       </c>
@@ -3345,14 +3634,17 @@
         <v>0</v>
       </c>
       <c r="BD14" s="7"/>
-      <c r="BE14" s="12">
+      <c r="BO14">
+        <v>1</v>
+      </c>
+      <c r="CI14" s="12">
         <v>73</v>
       </c>
-      <c r="BF14" s="1">
+      <c r="CJ14" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>58</v>
       </c>
@@ -3519,14 +3811,17 @@
         <v>0</v>
       </c>
       <c r="BD15" s="7"/>
-      <c r="BE15" s="12">
+      <c r="BY15">
+        <v>1</v>
+      </c>
+      <c r="CI15" s="12">
         <v>56</v>
       </c>
-      <c r="BF15" s="1">
+      <c r="CJ15" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>59</v>
       </c>
@@ -3693,14 +3988,17 @@
         <v>0</v>
       </c>
       <c r="BD16" s="7"/>
-      <c r="BE16" s="12">
+      <c r="BP16">
+        <v>1</v>
+      </c>
+      <c r="CI16" s="12">
         <v>15</v>
       </c>
-      <c r="BF16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="CJ16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>60</v>
       </c>
@@ -3867,14 +4165,17 @@
         <v>0</v>
       </c>
       <c r="BD17" s="7"/>
-      <c r="BE17" s="12">
+      <c r="BY17">
+        <v>1</v>
+      </c>
+      <c r="CI17" s="12">
         <v>59</v>
       </c>
-      <c r="BF17" s="1">
+      <c r="CJ17" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>61</v>
       </c>
@@ -4041,14 +4342,17 @@
         <v>0</v>
       </c>
       <c r="BD18" s="7"/>
-      <c r="BE18" s="12">
+      <c r="BO18">
+        <v>1</v>
+      </c>
+      <c r="CI18" s="12">
         <v>73</v>
       </c>
-      <c r="BF18" s="1">
+      <c r="CJ18" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>62</v>
       </c>
@@ -4215,14 +4519,17 @@
         <v>0</v>
       </c>
       <c r="BD19" s="7"/>
-      <c r="BE19" s="12">
+      <c r="BI19">
+        <v>1</v>
+      </c>
+      <c r="CI19" s="12">
         <v>73</v>
       </c>
-      <c r="BF19" s="1">
+      <c r="CJ19" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>63</v>
       </c>
@@ -4389,14 +4696,17 @@
         <v>0</v>
       </c>
       <c r="BD20" s="7"/>
-      <c r="BE20" s="12">
+      <c r="BY20">
+        <v>1</v>
+      </c>
+      <c r="CI20" s="12">
         <v>70</v>
       </c>
-      <c r="BF20" s="1">
+      <c r="CJ20" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>64</v>
       </c>
@@ -4563,14 +4873,17 @@
         <v>0</v>
       </c>
       <c r="BD21" s="7"/>
-      <c r="BE21" s="12">
+      <c r="BZ21">
+        <v>1</v>
+      </c>
+      <c r="CI21" s="12">
         <v>56</v>
       </c>
-      <c r="BF21" s="1">
+      <c r="CJ21" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>65</v>
       </c>
@@ -4737,14 +5050,17 @@
         <v>0</v>
       </c>
       <c r="BD22" s="7"/>
-      <c r="BE22" s="12">
+      <c r="BY22">
+        <v>1</v>
+      </c>
+      <c r="CI22" s="12">
         <v>29</v>
       </c>
-      <c r="BF22" s="1">
+      <c r="CJ22" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>66</v>
       </c>
@@ -4911,14 +5227,17 @@
         <v>0</v>
       </c>
       <c r="BD23" s="7"/>
-      <c r="BE23" s="12">
+      <c r="BY23">
+        <v>1</v>
+      </c>
+      <c r="CI23" s="12">
         <v>29</v>
       </c>
-      <c r="BF23" s="1">
+      <c r="CJ23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>67</v>
       </c>
@@ -5085,14 +5404,14 @@
         <v>0</v>
       </c>
       <c r="BD24" s="7"/>
-      <c r="BE24" s="12">
+      <c r="CI24" s="12">
         <v>73</v>
       </c>
-      <c r="BF24" s="1">
+      <c r="CJ24" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>68</v>
       </c>
@@ -5259,14 +5578,17 @@
         <v>0</v>
       </c>
       <c r="BD25" s="7"/>
-      <c r="BE25" s="12">
+      <c r="BO25">
+        <v>1</v>
+      </c>
+      <c r="CI25" s="12">
         <v>73</v>
       </c>
-      <c r="BF25" s="1">
+      <c r="CJ25" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>69</v>
       </c>
@@ -5433,14 +5755,17 @@
         <v>0</v>
       </c>
       <c r="BD26" s="7"/>
-      <c r="BE26" s="12">
+      <c r="BY26">
+        <v>1</v>
+      </c>
+      <c r="CI26" s="12">
         <v>41</v>
       </c>
-      <c r="BF26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="CJ26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>70</v>
       </c>
@@ -5607,14 +5932,17 @@
         <v>0</v>
       </c>
       <c r="BD27" s="7"/>
-      <c r="BE27" s="12">
+      <c r="BY27">
+        <v>1</v>
+      </c>
+      <c r="CI27" s="12">
         <v>15</v>
       </c>
-      <c r="BF27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="CJ27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>71</v>
       </c>
@@ -5781,10 +6109,24 @@
         <v>0</v>
       </c>
       <c r="BD28" s="7"/>
-      <c r="BE28" s="12">
+      <c r="CF28">
+        <v>1</v>
+      </c>
+      <c r="CI28" s="12">
         <v>55</v>
       </c>
-      <c r="BF28" s="1">
+      <c r="CJ28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="AF32">
+        <v>1</v>
+      </c>
+      <c r="AH32">
+        <v>1</v>
+      </c>
+      <c r="AI32">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor changes to forage_plant_location.xlxs and butterfly matrix spreadsheet
</commit_message>
<xml_diff>
--- a/Butterfly matrix.xlsx
+++ b/Butterfly matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBF1040-CAE7-154E-8A8D-B24BE49476D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BDCB31-AF47-6E4E-A7EF-C8CC21F8B627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1273,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ32"/>
+  <dimension ref="A1:CJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="AW6" sqref="AW6"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AF32" sqref="AF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6119,17 +6119,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="AF32">
-        <v>1</v>
-      </c>
-      <c r="AH32">
-        <v>1</v>
-      </c>
-      <c r="AI32">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="AY2:BC2"/>

</xml_diff>

<commit_message>
correct number of generations in butterfy matrix
</commit_message>
<xml_diff>
--- a/Butterfly matrix.xlsx
+++ b/Butterfly matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BDCB31-AF47-6E4E-A7EF-C8CC21F8B627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6BB169-DCEA-B34A-B904-31D16A6F49EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,6 +45,7 @@
     <author>tc={064B13DD-90E0-8F45-B29A-F1CD0F9FA9F0}</author>
     <author>tc={31CD7082-096C-F146-AD37-5C05666D3194}</author>
     <author>tc={474050C6-30EB-3142-8B55-53BB5FF6866F}</author>
+    <author>tc={33FF3A70-4CB3-A240-BDFC-FA10D8E6DB73}</author>
   </authors>
   <commentList>
     <comment ref="CI4" authorId="0" shapeId="0" xr:uid="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
@@ -68,16 +69,16 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    3 in good years, 1 in the north + scotland</t>
+    3 adult gens in good years, 1 in the north + scotland</t>
       </text>
     </comment>
     <comment ref="D11" authorId="3" shapeId="0" xr:uid="{15BF380F-61B2-E941-ACCA-2C49C8A69440}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     1 in north + high alt
-</t>
+3 in good years</t>
       </text>
     </comment>
     <comment ref="D12" authorId="4" shapeId="0" xr:uid="{9E270E82-241A-A34D-929E-62B5CB62F271}">
@@ -103,7 +104,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    can be 2, esp in north</t>
+    can be 2 adult, 3 lark, esp in north. in good years can be 4th adult gen</t>
       </text>
     </comment>
     <comment ref="D22" authorId="7" shapeId="0" xr:uid="{ECF40402-DD79-494B-8824-170BD6491CD4}">
@@ -119,7 +120,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    1 in north</t>
+    2 in north</t>
       </text>
     </comment>
     <comment ref="D25" authorId="9" shapeId="0" xr:uid="{31CD7082-096C-F146-AD37-5C05666D3194}">
@@ -138,6 +139,14 @@
     can also be 2 depending on conditions </t>
       </text>
     </comment>
+    <comment ref="D27" authorId="11" shapeId="0" xr:uid="{33FF3A70-4CB3-A240-BDFC-FA10D8E6DB73}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    3rd adult gen in good years</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -611,7 +620,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -637,6 +646,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1239,11 +1254,11 @@
     <text>This is Fl</text>
   </threadedComment>
   <threadedComment ref="E8" dT="2021-04-15T18:05:37.40" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{C66782A8-B31B-4B41-ABAC-0834AB6DC62E}">
-    <text>3 in good years, 1 in the north + scotland</text>
+    <text>3 adult gens in good years, 1 in the north + scotland</text>
   </threadedComment>
   <threadedComment ref="D11" dT="2021-04-15T20:15:18.97" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{15BF380F-61B2-E941-ACCA-2C49C8A69440}">
-    <text xml:space="preserve">1 in north + high alt
-</text>
+    <text>1 in north + high alt
+3 in good years</text>
   </threadedComment>
   <threadedComment ref="D12" dT="2021-04-15T20:16:56.66" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{9E270E82-241A-A34D-929E-62B5CB62F271}">
     <text xml:space="preserve">can be 3, 1 in north
@@ -1254,19 +1269,22 @@
 </text>
   </threadedComment>
   <threadedComment ref="D21" dT="2021-04-15T20:31:10.71" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{51C13814-482B-F046-9AB6-27C4D684F0D1}">
-    <text>can be 2, esp in north</text>
+    <text>can be 2 adult, 3 lark, esp in north. in good years can be 4th adult gen</text>
   </threadedComment>
   <threadedComment ref="D22" dT="2021-04-15T20:34:28.45" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{ECF40402-DD79-494B-8824-170BD6491CD4}">
     <text>3 in good years, 1 in north</text>
   </threadedComment>
   <threadedComment ref="D24" dT="2021-04-15T20:47:15.57" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{064B13DD-90E0-8F45-B29A-F1CD0F9FA9F0}">
-    <text>1 in north</text>
+    <text>2 in north</text>
   </threadedComment>
   <threadedComment ref="D25" dT="2021-04-15T20:48:37.48" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{31CD7082-096C-F146-AD37-5C05666D3194}">
     <text>3 in good years</text>
   </threadedComment>
   <threadedComment ref="D26" dT="2021-04-15T20:59:12.16" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{474050C6-30EB-3142-8B55-53BB5FF6866F}">
     <text xml:space="preserve">can also be 2 depending on conditions </text>
+  </threadedComment>
+  <threadedComment ref="D27" dT="2021-04-20T17:56:29.66" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{33FF3A70-4CB3-A240-BDFC-FA10D8E6DB73}">
+    <text>3rd adult gen in good years</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1275,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AF32" sqref="AF32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2212,7 +2230,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -2401,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="8">
         <v>1</v>
@@ -2756,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="8">
         <v>1</v>
@@ -3304,7 +3322,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="8">
         <v>0</v>
@@ -3658,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="8">
         <v>1</v>
@@ -4012,7 +4030,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="8">
         <v>1</v>
@@ -4363,7 +4381,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -4543,7 +4561,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="8">
         <v>1</v>
@@ -4720,7 +4738,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F21" s="8">
         <v>1</v>
@@ -5074,7 +5092,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="8">
         <v>0</v>
@@ -5248,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
@@ -5779,7 +5797,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
tried out or-ing each activity period, changed back as didn't work
</commit_message>
<xml_diff>
--- a/Butterfly matrix.xlsx
+++ b/Butterfly matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C28A1F1-2319-D94E-9F40-384C5019ECAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E3780F-B0EC-0C48-B80A-88705A196423}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,7 +656,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,12 +682,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -907,33 +901,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -959,6 +926,33 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1352,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1:AK1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1362,13 +1356,13 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="43" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="34" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="9" max="9" width="9.83203125" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="43" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="34" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" customWidth="1"/>
     <col min="17" max="17" width="10.83203125" customWidth="1"/>
     <col min="18" max="19" width="9.83203125" customWidth="1"/>
@@ -1376,24 +1370,24 @@
     <col min="21" max="22" width="9.83203125" customWidth="1"/>
     <col min="23" max="23" width="10.6640625" customWidth="1"/>
     <col min="24" max="26" width="9.83203125" customWidth="1"/>
-    <col min="29" max="30" width="8.83203125" style="43"/>
+    <col min="29" max="30" width="8.83203125" style="34"/>
     <col min="31" max="31" width="10.5" customWidth="1"/>
     <col min="32" max="32" width="12.5" customWidth="1"/>
     <col min="33" max="33" width="12.83203125" customWidth="1"/>
     <col min="34" max="34" width="11.6640625" customWidth="1"/>
     <col min="35" max="35" width="12.6640625" customWidth="1"/>
-    <col min="36" max="36" width="9.5" style="43" customWidth="1"/>
-    <col min="37" max="37" width="9.1640625" style="43" customWidth="1"/>
+    <col min="36" max="36" width="9.5" style="34" customWidth="1"/>
+    <col min="37" max="37" width="9.1640625" style="34" customWidth="1"/>
     <col min="40" max="40" width="9.83203125" customWidth="1"/>
-    <col min="43" max="44" width="8.83203125" style="43"/>
+    <col min="43" max="44" width="8.83203125" style="34"/>
     <col min="51" max="51" width="9.83203125" customWidth="1"/>
     <col min="54" max="54" width="10.33203125" customWidth="1"/>
-    <col min="60" max="61" width="8.83203125" style="43"/>
+    <col min="60" max="61" width="8.83203125" style="34"/>
     <col min="63" max="63" width="10.5" customWidth="1"/>
     <col min="64" max="64" width="10.1640625" customWidth="1"/>
     <col min="65" max="65" width="11" customWidth="1"/>
     <col min="66" max="66" width="10.1640625" customWidth="1"/>
-    <col min="67" max="67" width="10.83203125" style="43" customWidth="1"/>
+    <col min="67" max="67" width="10.83203125" style="34" customWidth="1"/>
     <col min="99" max="99" width="17.6640625" customWidth="1"/>
     <col min="100" max="100" width="19.6640625" customWidth="1"/>
   </cols>
@@ -1401,175 +1395,175 @@
     <row r="1" spans="1:100" x14ac:dyDescent="0.2">
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="36" t="s">
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
-      <c r="AO1" s="36"/>
-      <c r="AP1" s="36"/>
-      <c r="AQ1" s="36"/>
-      <c r="AR1" s="36"/>
-      <c r="AS1" s="36"/>
-      <c r="AT1" s="36"/>
-      <c r="AU1" s="36"/>
-      <c r="AV1" s="36"/>
-      <c r="AW1" s="36"/>
-      <c r="AX1" s="36"/>
-      <c r="AY1" s="36"/>
-      <c r="AZ1" s="36"/>
-      <c r="BA1" s="36"/>
-      <c r="BB1" s="36"/>
-      <c r="BC1" s="36"/>
-      <c r="BD1" s="36"/>
-      <c r="BE1" s="36"/>
-      <c r="BF1" s="36"/>
-      <c r="BG1" s="36"/>
-      <c r="BH1" s="36"/>
-      <c r="BI1" s="36"/>
-      <c r="BJ1" s="36"/>
-      <c r="BK1" s="36"/>
-      <c r="BL1" s="36"/>
-      <c r="BM1" s="36"/>
-      <c r="BN1" s="36"/>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="42"/>
-      <c r="BQ1" s="42"/>
-      <c r="BR1" s="42"/>
-      <c r="BS1" s="42"/>
-      <c r="BT1" s="42"/>
-      <c r="BU1" s="42"/>
-      <c r="BV1" s="42"/>
-      <c r="BW1" s="42"/>
-      <c r="BX1" s="42"/>
-      <c r="BY1" s="42"/>
-      <c r="BZ1" s="42"/>
-      <c r="CA1" s="42"/>
-      <c r="CB1" s="42"/>
-      <c r="CC1" s="42"/>
-      <c r="CD1" s="42"/>
-      <c r="CE1" s="42"/>
-      <c r="CF1" s="42"/>
-      <c r="CG1" s="42"/>
-      <c r="CH1" s="42"/>
-      <c r="CI1" s="42"/>
-      <c r="CJ1" s="42"/>
-      <c r="CK1" s="42"/>
-      <c r="CL1" s="42"/>
-      <c r="CM1" s="42"/>
-      <c r="CN1" s="42"/>
-      <c r="CO1" s="42"/>
-      <c r="CP1" s="42"/>
-      <c r="CQ1" s="42"/>
-      <c r="CR1" s="42"/>
-      <c r="CS1" s="42"/>
-      <c r="CT1" s="42"/>
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
+      <c r="BL1" s="45"/>
+      <c r="BM1" s="45"/>
+      <c r="BN1" s="45"/>
+      <c r="BO1" s="37"/>
+      <c r="BP1" s="33"/>
+      <c r="BQ1" s="33"/>
+      <c r="BR1" s="33"/>
+      <c r="BS1" s="33"/>
+      <c r="BT1" s="33"/>
+      <c r="BU1" s="33"/>
+      <c r="BV1" s="33"/>
+      <c r="BW1" s="33"/>
+      <c r="BX1" s="33"/>
+      <c r="BY1" s="33"/>
+      <c r="BZ1" s="33"/>
+      <c r="CA1" s="33"/>
+      <c r="CB1" s="33"/>
+      <c r="CC1" s="33"/>
+      <c r="CD1" s="33"/>
+      <c r="CE1" s="33"/>
+      <c r="CF1" s="33"/>
+      <c r="CG1" s="33"/>
+      <c r="CH1" s="33"/>
+      <c r="CI1" s="33"/>
+      <c r="CJ1" s="33"/>
+      <c r="CK1" s="33"/>
+      <c r="CL1" s="33"/>
+      <c r="CM1" s="33"/>
+      <c r="CN1" s="33"/>
+      <c r="CO1" s="33"/>
+      <c r="CP1" s="33"/>
+      <c r="CQ1" s="33"/>
+      <c r="CR1" s="33"/>
+      <c r="CS1" s="33"/>
+      <c r="CT1" s="33"/>
     </row>
     <row r="2" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="N2" s="38" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="N2" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="32" t="s">
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="47"/>
-      <c r="AK2" s="47"/>
-      <c r="AL2" s="37" t="s">
+      <c r="AF2" s="42"/>
+      <c r="AG2" s="42"/>
+      <c r="AH2" s="42"/>
+      <c r="AI2" s="42"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="38" t="s">
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="AT2" s="38"/>
-      <c r="AU2" s="38"/>
-      <c r="AV2" s="38"/>
-      <c r="AW2" s="38"/>
-      <c r="AX2" s="38"/>
-      <c r="AY2" s="38"/>
-      <c r="AZ2" s="38"/>
-      <c r="BA2" s="38"/>
-      <c r="BB2" s="38"/>
-      <c r="BC2" s="38"/>
-      <c r="BD2" s="38"/>
-      <c r="BE2" s="38"/>
-      <c r="BF2" s="38"/>
-      <c r="BG2" s="38"/>
-      <c r="BH2" s="46"/>
-      <c r="BI2" s="46"/>
-      <c r="BJ2" s="32" t="s">
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
+      <c r="AW2" s="47"/>
+      <c r="AX2" s="47"/>
+      <c r="AY2" s="47"/>
+      <c r="AZ2" s="47"/>
+      <c r="BA2" s="47"/>
+      <c r="BB2" s="47"/>
+      <c r="BC2" s="47"/>
+      <c r="BD2" s="47"/>
+      <c r="BE2" s="47"/>
+      <c r="BF2" s="47"/>
+      <c r="BG2" s="47"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="BK2" s="32"/>
-      <c r="BL2" s="32"/>
-      <c r="BM2" s="32"/>
-      <c r="BN2" s="32"/>
-      <c r="BO2" s="46"/>
+      <c r="BK2" s="41"/>
+      <c r="BL2" s="41"/>
+      <c r="BM2" s="41"/>
+      <c r="BN2" s="41"/>
+      <c r="BO2" s="37"/>
     </row>
     <row r="3" spans="1:100" x14ac:dyDescent="0.2">
       <c r="G3" s="14" t="s">
@@ -1587,33 +1581,33 @@
       <c r="K3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="31" t="s">
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="30" t="s">
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="31" t="s">
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="30" t="s">
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="47"/>
-      <c r="AD3" s="47"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
       <c r="AE3" s="21" t="s">
         <v>99</v>
       </c>
@@ -1629,8 +1623,8 @@
       <c r="AI3" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="AJ3" s="47"/>
-      <c r="AK3" s="47"/>
+      <c r="AJ3" s="38"/>
+      <c r="AK3" s="38"/>
       <c r="AL3" s="14" t="s">
         <v>99</v>
       </c>
@@ -1646,35 +1640,35 @@
       <c r="AP3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="AQ3" s="47"/>
-      <c r="AR3" s="47"/>
-      <c r="AS3" s="30" t="s">
+      <c r="AQ3" s="38"/>
+      <c r="AR3" s="38"/>
+      <c r="AS3" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="AT3" s="30"/>
-      <c r="AU3" s="30"/>
-      <c r="AV3" s="31" t="s">
+      <c r="AT3" s="48"/>
+      <c r="AU3" s="48"/>
+      <c r="AV3" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="AW3" s="31"/>
-      <c r="AX3" s="31"/>
-      <c r="AY3" s="30" t="s">
+      <c r="AW3" s="49"/>
+      <c r="AX3" s="49"/>
+      <c r="AY3" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="AZ3" s="30"/>
-      <c r="BA3" s="30"/>
-      <c r="BB3" s="31" t="s">
+      <c r="AZ3" s="48"/>
+      <c r="BA3" s="48"/>
+      <c r="BB3" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="BC3" s="31"/>
-      <c r="BD3" s="31"/>
-      <c r="BE3" s="30" t="s">
+      <c r="BC3" s="49"/>
+      <c r="BD3" s="49"/>
+      <c r="BE3" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="BF3" s="30"/>
-      <c r="BG3" s="30"/>
-      <c r="BH3" s="47"/>
-      <c r="BI3" s="47"/>
+      <c r="BF3" s="48"/>
+      <c r="BG3" s="48"/>
+      <c r="BH3" s="38"/>
+      <c r="BI3" s="38"/>
       <c r="BJ3" s="21" t="s">
         <v>99</v>
       </c>
@@ -1690,7 +1684,7 @@
       <c r="BN3" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="BO3" s="47"/>
+      <c r="BO3" s="38"/>
     </row>
     <row r="4" spans="1:100" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1708,7 +1702,7 @@
       <c r="E4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="35" t="s">
         <v>154</v>
       </c>
       <c r="G4" s="15" t="s">
@@ -1726,10 +1720,10 @@
       <c r="K4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="L4" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="36" t="s">
         <v>156</v>
       </c>
       <c r="N4" s="19" t="s">
@@ -1777,10 +1771,10 @@
       <c r="AB4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AC4" s="48" t="s">
+      <c r="AC4" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="AD4" s="48" t="s">
+      <c r="AD4" s="39" t="s">
         <v>158</v>
       </c>
       <c r="AE4" s="22" t="s">
@@ -1798,10 +1792,10 @@
       <c r="AI4" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="AJ4" s="48" t="s">
+      <c r="AJ4" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="AK4" s="48" t="s">
+      <c r="AK4" s="39" t="s">
         <v>160</v>
       </c>
       <c r="AL4" s="25" t="s">
@@ -1819,10 +1813,10 @@
       <c r="AP4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AQ4" s="48" t="s">
+      <c r="AQ4" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="AR4" s="48" t="s">
+      <c r="AR4" s="39" t="s">
         <v>162</v>
       </c>
       <c r="AS4" s="19" t="s">
@@ -1870,10 +1864,10 @@
       <c r="BG4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="BH4" s="48" t="s">
+      <c r="BH4" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="BI4" s="48" t="s">
+      <c r="BI4" s="39" t="s">
         <v>164</v>
       </c>
       <c r="BJ4" s="22" t="s">
@@ -1891,100 +1885,100 @@
       <c r="BN4" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="BO4" s="48" t="s">
+      <c r="BO4" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="BP4" s="39" t="s">
+      <c r="BP4" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="BQ4" s="39" t="s">
+      <c r="BQ4" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="BR4" s="40" t="s">
+      <c r="BR4" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="BS4" s="39" t="s">
+      <c r="BS4" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="BT4" s="39" t="s">
+      <c r="BT4" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="BU4" s="39" t="s">
+      <c r="BU4" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="BV4" s="39" t="s">
+      <c r="BV4" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="BW4" s="39" t="s">
+      <c r="BW4" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="BX4" s="39" t="s">
+      <c r="BX4" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="BY4" s="39" t="s">
+      <c r="BY4" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="BZ4" s="39" t="s">
+      <c r="BZ4" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="CA4" s="39" t="s">
+      <c r="CA4" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="CB4" s="39" t="s">
+      <c r="CB4" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="CC4" s="39" t="s">
+      <c r="CC4" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="CD4" s="39" t="s">
+      <c r="CD4" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="CE4" s="39" t="s">
+      <c r="CE4" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="CF4" s="39" t="s">
+      <c r="CF4" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="CG4" s="39" t="s">
+      <c r="CG4" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="CH4" s="39" t="s">
+      <c r="CH4" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="CI4" s="39" t="s">
+      <c r="CI4" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="CJ4" s="39" t="s">
+      <c r="CJ4" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="CK4" s="39" t="s">
+      <c r="CK4" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="CL4" s="39" t="s">
+      <c r="CL4" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="CM4" s="39" t="s">
+      <c r="CM4" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="CN4" s="39" t="s">
+      <c r="CN4" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="CO4" s="39" t="s">
+      <c r="CO4" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="CP4" s="39" t="s">
+      <c r="CP4" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="CQ4" s="39" t="s">
+      <c r="CQ4" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="CR4" s="39" t="s">
+      <c r="CR4" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="CS4" s="39" t="s">
+      <c r="CS4" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="CT4" s="39" t="s">
+      <c r="CT4" s="30" t="s">
         <v>152</v>
       </c>
       <c r="CU4" s="6" t="s">
@@ -2010,7 +2004,7 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="44"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8">
         <v>1</v>
       </c>
@@ -2026,8 +2020,8 @@
       <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
       <c r="N5" s="10">
         <v>1</v>
       </c>
@@ -2073,8 +2067,8 @@
       <c r="AB5" s="7">
         <v>1</v>
       </c>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="35"/>
       <c r="AE5" s="7">
         <v>1</v>
       </c>
@@ -2090,8 +2084,8 @@
       <c r="AI5" s="7">
         <v>1</v>
       </c>
-      <c r="AJ5" s="44"/>
-      <c r="AK5" s="44"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
       <c r="AL5" s="11">
         <v>1</v>
       </c>
@@ -2107,8 +2101,8 @@
       <c r="AP5" s="10">
         <v>0</v>
       </c>
-      <c r="AQ5" s="49"/>
-      <c r="AR5" s="49"/>
+      <c r="AQ5" s="40"/>
+      <c r="AR5" s="40"/>
       <c r="AS5" s="7">
         <v>0</v>
       </c>
@@ -2154,8 +2148,8 @@
       <c r="BG5" s="7">
         <v>0</v>
       </c>
-      <c r="BH5" s="44"/>
-      <c r="BI5" s="44"/>
+      <c r="BH5" s="35"/>
+      <c r="BI5" s="35"/>
       <c r="BJ5" s="7">
         <v>1</v>
       </c>
@@ -2171,9 +2165,9 @@
       <c r="BN5" s="7">
         <v>0</v>
       </c>
-      <c r="BO5" s="44"/>
-      <c r="BQ5" s="39"/>
-      <c r="BR5" s="39"/>
+      <c r="BO5" s="35"/>
+      <c r="BQ5" s="30"/>
+      <c r="BR5" s="30"/>
       <c r="CN5">
         <v>1</v>
       </c>
@@ -2200,7 +2194,7 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="44"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="8">
         <v>1</v>
       </c>
@@ -2216,8 +2210,8 @@
       <c r="K6" s="9">
         <v>0</v>
       </c>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
       <c r="N6" s="10">
         <v>0</v>
       </c>
@@ -2263,8 +2257,8 @@
       <c r="AB6" s="7">
         <v>0</v>
       </c>
-      <c r="AC6" s="44"/>
-      <c r="AD6" s="44"/>
+      <c r="AC6" s="35"/>
+      <c r="AD6" s="35"/>
       <c r="AE6" s="7">
         <v>1</v>
       </c>
@@ -2280,8 +2274,8 @@
       <c r="AI6" s="7">
         <v>0</v>
       </c>
-      <c r="AJ6" s="44"/>
-      <c r="AK6" s="44"/>
+      <c r="AJ6" s="35"/>
+      <c r="AK6" s="35"/>
       <c r="AL6" s="11">
         <v>1</v>
       </c>
@@ -2297,8 +2291,8 @@
       <c r="AP6" s="10">
         <v>0</v>
       </c>
-      <c r="AQ6" s="49"/>
-      <c r="AR6" s="49"/>
+      <c r="AQ6" s="40"/>
+      <c r="AR6" s="40"/>
       <c r="AS6" s="7">
         <v>1</v>
       </c>
@@ -2344,8 +2338,8 @@
       <c r="BG6" s="7">
         <v>0</v>
       </c>
-      <c r="BH6" s="44"/>
-      <c r="BI6" s="44"/>
+      <c r="BH6" s="35"/>
+      <c r="BI6" s="35"/>
       <c r="BJ6" s="7">
         <v>0</v>
       </c>
@@ -2361,10 +2355,10 @@
       <c r="BN6" s="7">
         <v>0</v>
       </c>
-      <c r="BO6" s="44"/>
-      <c r="BQ6" s="40"/>
-      <c r="BR6" s="40"/>
-      <c r="CN6" s="41"/>
+      <c r="BO6" s="35"/>
+      <c r="BQ6" s="31"/>
+      <c r="BR6" s="31"/>
+      <c r="CN6" s="32"/>
       <c r="CO6">
         <v>1</v>
       </c>
@@ -2391,7 +2385,7 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="44"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="8">
         <v>1</v>
       </c>
@@ -2407,8 +2401,8 @@
       <c r="K7" s="9">
         <v>1</v>
       </c>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
       <c r="N7" s="10">
         <v>1</v>
       </c>
@@ -2454,8 +2448,8 @@
       <c r="AB7" s="7">
         <v>1</v>
       </c>
-      <c r="AC7" s="44"/>
-      <c r="AD7" s="44"/>
+      <c r="AC7" s="35"/>
+      <c r="AD7" s="35"/>
       <c r="AE7" s="7">
         <v>1</v>
       </c>
@@ -2471,8 +2465,8 @@
       <c r="AI7" s="7">
         <v>1</v>
       </c>
-      <c r="AJ7" s="44"/>
-      <c r="AK7" s="44"/>
+      <c r="AJ7" s="35"/>
+      <c r="AK7" s="35"/>
       <c r="AL7" s="11">
         <v>1</v>
       </c>
@@ -2488,8 +2482,8 @@
       <c r="AP7" s="10">
         <v>0</v>
       </c>
-      <c r="AQ7" s="49"/>
-      <c r="AR7" s="49"/>
+      <c r="AQ7" s="40"/>
+      <c r="AR7" s="40"/>
       <c r="AS7" s="7">
         <v>1</v>
       </c>
@@ -2535,8 +2529,8 @@
       <c r="BG7" s="7">
         <v>0</v>
       </c>
-      <c r="BH7" s="44"/>
-      <c r="BI7" s="44"/>
+      <c r="BH7" s="35"/>
+      <c r="BI7" s="35"/>
       <c r="BJ7" s="7">
         <v>1</v>
       </c>
@@ -2552,7 +2546,7 @@
       <c r="BN7" s="7">
         <v>0</v>
       </c>
-      <c r="BO7" s="44"/>
+      <c r="BO7" s="35"/>
       <c r="BP7" s="7"/>
       <c r="BU7">
         <v>1</v>
@@ -2589,7 +2583,7 @@
       <c r="E8" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="44"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="8">
         <v>1</v>
       </c>
@@ -2605,8 +2599,8 @@
       <c r="K8" s="9">
         <v>0</v>
       </c>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
       <c r="N8" s="10">
         <v>1</v>
       </c>
@@ -2652,8 +2646,8 @@
       <c r="AB8" s="7">
         <v>0</v>
       </c>
-      <c r="AC8" s="44"/>
-      <c r="AD8" s="44"/>
+      <c r="AC8" s="35"/>
+      <c r="AD8" s="35"/>
       <c r="AE8" s="7">
         <v>1</v>
       </c>
@@ -2669,8 +2663,8 @@
       <c r="AI8" s="7">
         <v>0</v>
       </c>
-      <c r="AJ8" s="44"/>
-      <c r="AK8" s="44"/>
+      <c r="AJ8" s="35"/>
+      <c r="AK8" s="35"/>
       <c r="AL8" s="11">
         <v>0</v>
       </c>
@@ -2686,8 +2680,8 @@
       <c r="AP8" s="10">
         <v>0</v>
       </c>
-      <c r="AQ8" s="49"/>
-      <c r="AR8" s="49"/>
+      <c r="AQ8" s="40"/>
+      <c r="AR8" s="40"/>
       <c r="AS8" s="7">
         <v>0</v>
       </c>
@@ -2733,8 +2727,8 @@
       <c r="BG8" s="7">
         <v>0</v>
       </c>
-      <c r="BH8" s="44"/>
-      <c r="BI8" s="44"/>
+      <c r="BH8" s="35"/>
+      <c r="BI8" s="35"/>
       <c r="BJ8" s="7">
         <v>0</v>
       </c>
@@ -2750,7 +2744,7 @@
       <c r="BN8" s="7">
         <v>0</v>
       </c>
-      <c r="BO8" s="44"/>
+      <c r="BO8" s="35"/>
       <c r="BP8" s="7"/>
       <c r="CC8">
         <v>1</v>
@@ -2778,7 +2772,7 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" s="44"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="8">
         <v>0</v>
       </c>
@@ -2794,8 +2788,8 @@
       <c r="K9" s="9">
         <v>0</v>
       </c>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
       <c r="N9" s="10">
         <v>0</v>
       </c>
@@ -2841,8 +2835,8 @@
       <c r="AB9" s="7">
         <v>0</v>
       </c>
-      <c r="AC9" s="44"/>
-      <c r="AD9" s="44"/>
+      <c r="AC9" s="35"/>
+      <c r="AD9" s="35"/>
       <c r="AE9" s="7">
         <v>0</v>
       </c>
@@ -2858,8 +2852,8 @@
       <c r="AI9" s="7">
         <v>0</v>
       </c>
-      <c r="AJ9" s="44"/>
-      <c r="AK9" s="44"/>
+      <c r="AJ9" s="35"/>
+      <c r="AK9" s="35"/>
       <c r="AL9" s="11">
         <v>0</v>
       </c>
@@ -2875,8 +2869,8 @@
       <c r="AP9" s="10">
         <v>0</v>
       </c>
-      <c r="AQ9" s="49"/>
-      <c r="AR9" s="49"/>
+      <c r="AQ9" s="40"/>
+      <c r="AR9" s="40"/>
       <c r="AS9" s="7">
         <v>0</v>
       </c>
@@ -2922,8 +2916,8 @@
       <c r="BG9" s="7">
         <v>0</v>
       </c>
-      <c r="BH9" s="44"/>
-      <c r="BI9" s="44"/>
+      <c r="BH9" s="35"/>
+      <c r="BI9" s="35"/>
       <c r="BJ9" s="7">
         <v>0</v>
       </c>
@@ -2939,9 +2933,9 @@
       <c r="BN9" s="7">
         <v>0</v>
       </c>
-      <c r="BO9" s="44"/>
+      <c r="BO9" s="35"/>
       <c r="BP9" s="7"/>
-      <c r="BV9" s="39"/>
+      <c r="BV9" s="30"/>
       <c r="CK9">
         <v>1</v>
       </c>
@@ -2968,7 +2962,7 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="F10" s="44"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="8">
         <v>1</v>
       </c>
@@ -2984,8 +2978,8 @@
       <c r="K10" s="9">
         <v>0</v>
       </c>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
       <c r="N10" s="10">
         <v>0</v>
       </c>
@@ -3031,8 +3025,8 @@
       <c r="AB10" s="7">
         <v>0</v>
       </c>
-      <c r="AC10" s="44"/>
-      <c r="AD10" s="44"/>
+      <c r="AC10" s="35"/>
+      <c r="AD10" s="35"/>
       <c r="AE10" s="7">
         <v>1</v>
       </c>
@@ -3048,8 +3042,8 @@
       <c r="AI10" s="7">
         <v>0</v>
       </c>
-      <c r="AJ10" s="44"/>
-      <c r="AK10" s="44"/>
+      <c r="AJ10" s="35"/>
+      <c r="AK10" s="35"/>
       <c r="AL10" s="11">
         <v>0</v>
       </c>
@@ -3065,8 +3059,8 @@
       <c r="AP10" s="10">
         <v>0</v>
       </c>
-      <c r="AQ10" s="49"/>
-      <c r="AR10" s="49"/>
+      <c r="AQ10" s="40"/>
+      <c r="AR10" s="40"/>
       <c r="AS10" s="7">
         <v>0</v>
       </c>
@@ -3112,8 +3106,8 @@
       <c r="BG10" s="7">
         <v>0</v>
       </c>
-      <c r="BH10" s="44"/>
-      <c r="BI10" s="44"/>
+      <c r="BH10" s="35"/>
+      <c r="BI10" s="35"/>
       <c r="BJ10" s="7">
         <v>0</v>
       </c>
@@ -3129,7 +3123,7 @@
       <c r="BN10" s="7">
         <v>0</v>
       </c>
-      <c r="BO10" s="44"/>
+      <c r="BO10" s="35"/>
       <c r="BP10" s="7"/>
       <c r="CK10">
         <v>1</v>
@@ -3157,7 +3151,7 @@
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="8">
         <v>1</v>
       </c>
@@ -3173,8 +3167,8 @@
       <c r="K11" s="9">
         <v>1</v>
       </c>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
       <c r="N11" s="10">
         <v>1</v>
       </c>
@@ -3220,8 +3214,8 @@
       <c r="AB11" s="7">
         <v>1</v>
       </c>
-      <c r="AC11" s="44"/>
-      <c r="AD11" s="44"/>
+      <c r="AC11" s="35"/>
+      <c r="AD11" s="35"/>
       <c r="AE11" s="7">
         <v>1</v>
       </c>
@@ -3237,8 +3231,8 @@
       <c r="AI11" s="7">
         <v>1</v>
       </c>
-      <c r="AJ11" s="44"/>
-      <c r="AK11" s="44"/>
+      <c r="AJ11" s="35"/>
+      <c r="AK11" s="35"/>
       <c r="AL11" s="11">
         <v>0</v>
       </c>
@@ -3254,8 +3248,8 @@
       <c r="AP11" s="10">
         <v>0</v>
       </c>
-      <c r="AQ11" s="49"/>
-      <c r="AR11" s="49"/>
+      <c r="AQ11" s="40"/>
+      <c r="AR11" s="40"/>
       <c r="AS11" s="7">
         <v>0</v>
       </c>
@@ -3301,8 +3295,8 @@
       <c r="BG11" s="7">
         <v>0</v>
       </c>
-      <c r="BH11" s="44"/>
-      <c r="BI11" s="44"/>
+      <c r="BH11" s="35"/>
+      <c r="BI11" s="35"/>
       <c r="BJ11" s="7">
         <v>0</v>
       </c>
@@ -3318,7 +3312,7 @@
       <c r="BN11" s="7">
         <v>0</v>
       </c>
-      <c r="BO11" s="44"/>
+      <c r="BO11" s="35"/>
       <c r="BP11" s="7"/>
       <c r="CA11">
         <v>1</v>
@@ -3346,7 +3340,7 @@
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" s="44"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="8">
         <v>1</v>
       </c>
@@ -3362,8 +3356,8 @@
       <c r="K12" s="9">
         <v>0</v>
       </c>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
       <c r="N12" s="10">
         <v>1</v>
       </c>
@@ -3409,8 +3403,8 @@
       <c r="AB12" s="7">
         <v>0</v>
       </c>
-      <c r="AC12" s="44"/>
-      <c r="AD12" s="44"/>
+      <c r="AC12" s="35"/>
+      <c r="AD12" s="35"/>
       <c r="AE12" s="7">
         <v>1</v>
       </c>
@@ -3426,8 +3420,8 @@
       <c r="AI12" s="7">
         <v>0</v>
       </c>
-      <c r="AJ12" s="44"/>
-      <c r="AK12" s="44"/>
+      <c r="AJ12" s="35"/>
+      <c r="AK12" s="35"/>
       <c r="AL12" s="11">
         <v>1</v>
       </c>
@@ -3443,8 +3437,8 @@
       <c r="AP12" s="10">
         <v>0</v>
       </c>
-      <c r="AQ12" s="49"/>
-      <c r="AR12" s="49"/>
+      <c r="AQ12" s="40"/>
+      <c r="AR12" s="40"/>
       <c r="AS12" s="7">
         <v>1</v>
       </c>
@@ -3490,8 +3484,8 @@
       <c r="BG12" s="7">
         <v>0</v>
       </c>
-      <c r="BH12" s="44"/>
-      <c r="BI12" s="44"/>
+      <c r="BH12" s="35"/>
+      <c r="BI12" s="35"/>
       <c r="BJ12" s="7">
         <v>0</v>
       </c>
@@ -3507,7 +3501,7 @@
       <c r="BN12" s="7">
         <v>0</v>
       </c>
-      <c r="BO12" s="44"/>
+      <c r="BO12" s="35"/>
       <c r="BP12" s="1">
         <v>1</v>
       </c>
@@ -3552,7 +3546,7 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="44"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="8">
         <v>0</v>
       </c>
@@ -3568,8 +3562,8 @@
       <c r="K13" s="9">
         <v>0</v>
       </c>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
       <c r="N13" s="10">
         <v>0</v>
       </c>
@@ -3615,8 +3609,8 @@
       <c r="AB13" s="7">
         <v>0</v>
       </c>
-      <c r="AC13" s="44"/>
-      <c r="AD13" s="44"/>
+      <c r="AC13" s="35"/>
+      <c r="AD13" s="35"/>
       <c r="AE13" s="7">
         <v>0</v>
       </c>
@@ -3632,8 +3626,8 @@
       <c r="AI13" s="7">
         <v>0</v>
       </c>
-      <c r="AJ13" s="44"/>
-      <c r="AK13" s="44"/>
+      <c r="AJ13" s="35"/>
+      <c r="AK13" s="35"/>
       <c r="AL13" s="11">
         <v>0</v>
       </c>
@@ -3649,8 +3643,8 @@
       <c r="AP13" s="10">
         <v>0</v>
       </c>
-      <c r="AQ13" s="49"/>
-      <c r="AR13" s="49"/>
+      <c r="AQ13" s="40"/>
+      <c r="AR13" s="40"/>
       <c r="AS13" s="7">
         <v>0</v>
       </c>
@@ -3696,8 +3690,8 @@
       <c r="BG13" s="7">
         <v>0</v>
       </c>
-      <c r="BH13" s="44"/>
-      <c r="BI13" s="44"/>
+      <c r="BH13" s="35"/>
+      <c r="BI13" s="35"/>
       <c r="BJ13" s="7">
         <v>0</v>
       </c>
@@ -3713,7 +3707,7 @@
       <c r="BN13" s="7">
         <v>0</v>
       </c>
-      <c r="BO13" s="44"/>
+      <c r="BO13" s="35"/>
       <c r="BP13" s="7"/>
       <c r="CK13">
         <v>1</v>
@@ -3741,7 +3735,7 @@
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="44"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="8">
         <v>1</v>
       </c>
@@ -3757,8 +3751,8 @@
       <c r="K14" s="9">
         <v>1</v>
       </c>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
       <c r="N14" s="10">
         <v>1</v>
       </c>
@@ -3804,8 +3798,8 @@
       <c r="AB14" s="7">
         <v>1</v>
       </c>
-      <c r="AC14" s="44"/>
-      <c r="AD14" s="44"/>
+      <c r="AC14" s="35"/>
+      <c r="AD14" s="35"/>
       <c r="AE14" s="7">
         <v>1</v>
       </c>
@@ -3821,8 +3815,8 @@
       <c r="AI14" s="7">
         <v>1</v>
       </c>
-      <c r="AJ14" s="44"/>
-      <c r="AK14" s="44"/>
+      <c r="AJ14" s="35"/>
+      <c r="AK14" s="35"/>
       <c r="AL14" s="11">
         <v>0</v>
       </c>
@@ -3838,8 +3832,8 @@
       <c r="AP14" s="10">
         <v>0</v>
       </c>
-      <c r="AQ14" s="49"/>
-      <c r="AR14" s="49"/>
+      <c r="AQ14" s="40"/>
+      <c r="AR14" s="40"/>
       <c r="AS14" s="7">
         <v>0</v>
       </c>
@@ -3885,8 +3879,8 @@
       <c r="BG14" s="7">
         <v>0</v>
       </c>
-      <c r="BH14" s="44"/>
-      <c r="BI14" s="44"/>
+      <c r="BH14" s="35"/>
+      <c r="BI14" s="35"/>
       <c r="BJ14" s="7">
         <v>0</v>
       </c>
@@ -3902,7 +3896,7 @@
       <c r="BN14" s="7">
         <v>0</v>
       </c>
-      <c r="BO14" s="44"/>
+      <c r="BO14" s="35"/>
       <c r="BP14" s="7"/>
       <c r="CA14">
         <v>1</v>
@@ -3930,7 +3924,7 @@
       <c r="E15" s="1">
         <v>2</v>
       </c>
-      <c r="F15" s="44"/>
+      <c r="F15" s="35"/>
       <c r="G15" s="8">
         <v>1</v>
       </c>
@@ -3946,8 +3940,8 @@
       <c r="K15" s="9">
         <v>0</v>
       </c>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
       <c r="N15" s="10">
         <v>0</v>
       </c>
@@ -3993,8 +3987,8 @@
       <c r="AB15" s="7">
         <v>0</v>
       </c>
-      <c r="AC15" s="44"/>
-      <c r="AD15" s="44"/>
+      <c r="AC15" s="35"/>
+      <c r="AD15" s="35"/>
       <c r="AE15" s="7">
         <v>1</v>
       </c>
@@ -4010,8 +4004,8 @@
       <c r="AI15" s="7">
         <v>0</v>
       </c>
-      <c r="AJ15" s="44"/>
-      <c r="AK15" s="44"/>
+      <c r="AJ15" s="35"/>
+      <c r="AK15" s="35"/>
       <c r="AL15" s="11">
         <v>0</v>
       </c>
@@ -4027,8 +4021,8 @@
       <c r="AP15" s="10">
         <v>0</v>
       </c>
-      <c r="AQ15" s="49"/>
-      <c r="AR15" s="49"/>
+      <c r="AQ15" s="40"/>
+      <c r="AR15" s="40"/>
       <c r="AS15" s="7">
         <v>0</v>
       </c>
@@ -4074,8 +4068,8 @@
       <c r="BG15" s="7">
         <v>0</v>
       </c>
-      <c r="BH15" s="44"/>
-      <c r="BI15" s="44"/>
+      <c r="BH15" s="35"/>
+      <c r="BI15" s="35"/>
       <c r="BJ15" s="7">
         <v>0</v>
       </c>
@@ -4091,7 +4085,7 @@
       <c r="BN15" s="7">
         <v>0</v>
       </c>
-      <c r="BO15" s="44"/>
+      <c r="BO15" s="35"/>
       <c r="BP15" s="7"/>
       <c r="CK15">
         <v>1</v>
@@ -4119,7 +4113,7 @@
       <c r="E16" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="44"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="8">
         <v>0</v>
       </c>
@@ -4135,8 +4129,8 @@
       <c r="K16" s="9">
         <v>0</v>
       </c>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="10">
         <v>0</v>
       </c>
@@ -4182,8 +4176,8 @@
       <c r="AB16" s="7">
         <v>0</v>
       </c>
-      <c r="AC16" s="44"/>
-      <c r="AD16" s="44"/>
+      <c r="AC16" s="35"/>
+      <c r="AD16" s="35"/>
       <c r="AE16" s="7">
         <v>0</v>
       </c>
@@ -4199,8 +4193,8 @@
       <c r="AI16" s="7">
         <v>0</v>
       </c>
-      <c r="AJ16" s="44"/>
-      <c r="AK16" s="44"/>
+      <c r="AJ16" s="35"/>
+      <c r="AK16" s="35"/>
       <c r="AL16" s="11">
         <v>0</v>
       </c>
@@ -4216,8 +4210,8 @@
       <c r="AP16" s="10">
         <v>0</v>
       </c>
-      <c r="AQ16" s="49"/>
-      <c r="AR16" s="49"/>
+      <c r="AQ16" s="40"/>
+      <c r="AR16" s="40"/>
       <c r="AS16" s="7">
         <v>0</v>
       </c>
@@ -4263,8 +4257,8 @@
       <c r="BG16" s="7">
         <v>0</v>
       </c>
-      <c r="BH16" s="44"/>
-      <c r="BI16" s="44"/>
+      <c r="BH16" s="35"/>
+      <c r="BI16" s="35"/>
       <c r="BJ16" s="7">
         <v>0</v>
       </c>
@@ -4280,7 +4274,7 @@
       <c r="BN16" s="7">
         <v>0</v>
       </c>
-      <c r="BO16" s="44"/>
+      <c r="BO16" s="35"/>
       <c r="BP16" s="7"/>
       <c r="CB16">
         <v>1</v>
@@ -4308,7 +4302,7 @@
       <c r="E17" s="1">
         <v>2</v>
       </c>
-      <c r="F17" s="44"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="8">
         <v>1</v>
       </c>
@@ -4324,8 +4318,8 @@
       <c r="K17" s="9">
         <v>0</v>
       </c>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="10">
         <v>0</v>
       </c>
@@ -4371,8 +4365,8 @@
       <c r="AB17" s="7">
         <v>0</v>
       </c>
-      <c r="AC17" s="44"/>
-      <c r="AD17" s="44"/>
+      <c r="AC17" s="35"/>
+      <c r="AD17" s="35"/>
       <c r="AE17" s="7">
         <v>1</v>
       </c>
@@ -4388,8 +4382,8 @@
       <c r="AI17" s="7">
         <v>0</v>
       </c>
-      <c r="AJ17" s="44"/>
-      <c r="AK17" s="44"/>
+      <c r="AJ17" s="35"/>
+      <c r="AK17" s="35"/>
       <c r="AL17" s="11">
         <v>0</v>
       </c>
@@ -4405,8 +4399,8 @@
       <c r="AP17" s="10">
         <v>0</v>
       </c>
-      <c r="AQ17" s="49"/>
-      <c r="AR17" s="49"/>
+      <c r="AQ17" s="40"/>
+      <c r="AR17" s="40"/>
       <c r="AS17" s="7">
         <v>0</v>
       </c>
@@ -4452,8 +4446,8 @@
       <c r="BG17" s="7">
         <v>0</v>
       </c>
-      <c r="BH17" s="44"/>
-      <c r="BI17" s="44"/>
+      <c r="BH17" s="35"/>
+      <c r="BI17" s="35"/>
       <c r="BJ17" s="7">
         <v>0</v>
       </c>
@@ -4469,7 +4463,7 @@
       <c r="BN17" s="7">
         <v>0</v>
       </c>
-      <c r="BO17" s="44"/>
+      <c r="BO17" s="35"/>
       <c r="BP17" s="7"/>
       <c r="CK17">
         <v>1</v>
@@ -4497,7 +4491,7 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="44"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="8">
         <v>1</v>
       </c>
@@ -4513,8 +4507,8 @@
       <c r="K18" s="9">
         <v>1</v>
       </c>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="10">
         <v>1</v>
       </c>
@@ -4560,8 +4554,8 @@
       <c r="AB18" s="7">
         <v>0</v>
       </c>
-      <c r="AC18" s="44"/>
-      <c r="AD18" s="44"/>
+      <c r="AC18" s="35"/>
+      <c r="AD18" s="35"/>
       <c r="AE18" s="7">
         <v>1</v>
       </c>
@@ -4577,8 +4571,8 @@
       <c r="AI18" s="7">
         <v>1</v>
       </c>
-      <c r="AJ18" s="44"/>
-      <c r="AK18" s="44"/>
+      <c r="AJ18" s="35"/>
+      <c r="AK18" s="35"/>
       <c r="AL18" s="11">
         <v>0</v>
       </c>
@@ -4594,8 +4588,8 @@
       <c r="AP18" s="10">
         <v>1</v>
       </c>
-      <c r="AQ18" s="49"/>
-      <c r="AR18" s="49"/>
+      <c r="AQ18" s="40"/>
+      <c r="AR18" s="40"/>
       <c r="AS18" s="7">
         <v>0</v>
       </c>
@@ -4641,8 +4635,8 @@
       <c r="BG18" s="7">
         <v>0</v>
       </c>
-      <c r="BH18" s="44"/>
-      <c r="BI18" s="44"/>
+      <c r="BH18" s="35"/>
+      <c r="BI18" s="35"/>
       <c r="BJ18" s="7">
         <v>0</v>
       </c>
@@ -4658,7 +4652,7 @@
       <c r="BN18" s="7">
         <v>0</v>
       </c>
-      <c r="BO18" s="44"/>
+      <c r="BO18" s="35"/>
       <c r="BP18" s="7"/>
       <c r="CA18">
         <v>1</v>
@@ -4686,7 +4680,7 @@
       <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="44"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="8">
         <v>1</v>
       </c>
@@ -4702,8 +4696,8 @@
       <c r="K19" s="9">
         <v>1</v>
       </c>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="10">
         <v>1</v>
       </c>
@@ -4749,8 +4743,8 @@
       <c r="AB19" s="7">
         <v>1</v>
       </c>
-      <c r="AC19" s="44"/>
-      <c r="AD19" s="44"/>
+      <c r="AC19" s="35"/>
+      <c r="AD19" s="35"/>
       <c r="AE19" s="7">
         <v>1</v>
       </c>
@@ -4766,8 +4760,8 @@
       <c r="AI19" s="7">
         <v>1</v>
       </c>
-      <c r="AJ19" s="44"/>
-      <c r="AK19" s="44"/>
+      <c r="AJ19" s="35"/>
+      <c r="AK19" s="35"/>
       <c r="AL19" s="11">
         <v>0</v>
       </c>
@@ -4783,8 +4777,8 @@
       <c r="AP19" s="10">
         <v>0</v>
       </c>
-      <c r="AQ19" s="49"/>
-      <c r="AR19" s="49"/>
+      <c r="AQ19" s="40"/>
+      <c r="AR19" s="40"/>
       <c r="AS19" s="7">
         <v>0</v>
       </c>
@@ -4830,8 +4824,8 @@
       <c r="BG19" s="7">
         <v>0</v>
       </c>
-      <c r="BH19" s="44"/>
-      <c r="BI19" s="44"/>
+      <c r="BH19" s="35"/>
+      <c r="BI19" s="35"/>
       <c r="BJ19" s="7">
         <v>0</v>
       </c>
@@ -4847,7 +4841,7 @@
       <c r="BN19" s="7">
         <v>0</v>
       </c>
-      <c r="BO19" s="44"/>
+      <c r="BO19" s="35"/>
       <c r="BP19" s="7"/>
       <c r="BU19">
         <v>1</v>
@@ -4875,7 +4869,7 @@
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="44"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="8">
         <v>1</v>
       </c>
@@ -4891,8 +4885,8 @@
       <c r="K20" s="9">
         <v>1</v>
       </c>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="10">
         <v>0</v>
       </c>
@@ -4938,8 +4932,8 @@
       <c r="AB20" s="7">
         <v>0</v>
       </c>
-      <c r="AC20" s="44"/>
-      <c r="AD20" s="44"/>
+      <c r="AC20" s="35"/>
+      <c r="AD20" s="35"/>
       <c r="AE20" s="7">
         <v>1</v>
       </c>
@@ -4955,8 +4949,8 @@
       <c r="AI20" s="7">
         <v>1</v>
       </c>
-      <c r="AJ20" s="44"/>
-      <c r="AK20" s="44"/>
+      <c r="AJ20" s="35"/>
+      <c r="AK20" s="35"/>
       <c r="AL20" s="11">
         <v>0</v>
       </c>
@@ -4972,8 +4966,8 @@
       <c r="AP20" s="10">
         <v>1</v>
       </c>
-      <c r="AQ20" s="49"/>
-      <c r="AR20" s="49"/>
+      <c r="AQ20" s="40"/>
+      <c r="AR20" s="40"/>
       <c r="AS20" s="7">
         <v>0</v>
       </c>
@@ -5019,8 +5013,8 @@
       <c r="BG20" s="7">
         <v>0</v>
       </c>
-      <c r="BH20" s="44"/>
-      <c r="BI20" s="44"/>
+      <c r="BH20" s="35"/>
+      <c r="BI20" s="35"/>
       <c r="BJ20" s="7">
         <v>0</v>
       </c>
@@ -5036,7 +5030,7 @@
       <c r="BN20" s="7">
         <v>0</v>
       </c>
-      <c r="BO20" s="44"/>
+      <c r="BO20" s="35"/>
       <c r="BP20" s="7"/>
       <c r="CK20">
         <v>1</v>
@@ -5064,7 +5058,7 @@
       <c r="E21" s="1">
         <v>4</v>
       </c>
-      <c r="F21" s="44"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="8">
         <v>1</v>
       </c>
@@ -5080,8 +5074,8 @@
       <c r="K21" s="9">
         <v>0</v>
       </c>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
       <c r="N21" s="10">
         <v>1</v>
       </c>
@@ -5127,8 +5121,8 @@
       <c r="AB21" s="7">
         <v>0</v>
       </c>
-      <c r="AC21" s="44"/>
-      <c r="AD21" s="44"/>
+      <c r="AC21" s="35"/>
+      <c r="AD21" s="35"/>
       <c r="AE21" s="7">
         <v>1</v>
       </c>
@@ -5144,8 +5138,8 @@
       <c r="AI21" s="7">
         <v>0</v>
       </c>
-      <c r="AJ21" s="44"/>
-      <c r="AK21" s="44"/>
+      <c r="AJ21" s="35"/>
+      <c r="AK21" s="35"/>
       <c r="AL21" s="11">
         <v>0</v>
       </c>
@@ -5161,8 +5155,8 @@
       <c r="AP21" s="10">
         <v>0</v>
       </c>
-      <c r="AQ21" s="49"/>
-      <c r="AR21" s="49"/>
+      <c r="AQ21" s="40"/>
+      <c r="AR21" s="40"/>
       <c r="AS21" s="7">
         <v>0</v>
       </c>
@@ -5208,8 +5202,8 @@
       <c r="BG21" s="7">
         <v>0</v>
       </c>
-      <c r="BH21" s="44"/>
-      <c r="BI21" s="44"/>
+      <c r="BH21" s="35"/>
+      <c r="BI21" s="35"/>
       <c r="BJ21" s="7">
         <v>0</v>
       </c>
@@ -5225,7 +5219,7 @@
       <c r="BN21" s="7">
         <v>0</v>
       </c>
-      <c r="BO21" s="44"/>
+      <c r="BO21" s="35"/>
       <c r="BP21" s="7"/>
       <c r="CL21">
         <v>1</v>
@@ -5253,7 +5247,7 @@
       <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="F22" s="44"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="8">
         <v>0</v>
       </c>
@@ -5269,8 +5263,8 @@
       <c r="K22" s="9">
         <v>0</v>
       </c>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
       <c r="N22" s="10">
         <v>0</v>
       </c>
@@ -5316,8 +5310,8 @@
       <c r="AB22" s="7">
         <v>0</v>
       </c>
-      <c r="AC22" s="44"/>
-      <c r="AD22" s="44"/>
+      <c r="AC22" s="35"/>
+      <c r="AD22" s="35"/>
       <c r="AE22" s="7">
         <v>0</v>
       </c>
@@ -5333,8 +5327,8 @@
       <c r="AI22" s="7">
         <v>0</v>
       </c>
-      <c r="AJ22" s="44"/>
-      <c r="AK22" s="44"/>
+      <c r="AJ22" s="35"/>
+      <c r="AK22" s="35"/>
       <c r="AL22" s="11">
         <v>0</v>
       </c>
@@ -5350,8 +5344,8 @@
       <c r="AP22" s="10">
         <v>0</v>
       </c>
-      <c r="AQ22" s="49"/>
-      <c r="AR22" s="49"/>
+      <c r="AQ22" s="40"/>
+      <c r="AR22" s="40"/>
       <c r="AS22" s="7">
         <v>0</v>
       </c>
@@ -5397,8 +5391,8 @@
       <c r="BG22" s="7">
         <v>0</v>
       </c>
-      <c r="BH22" s="44"/>
-      <c r="BI22" s="44"/>
+      <c r="BH22" s="35"/>
+      <c r="BI22" s="35"/>
       <c r="BJ22" s="7">
         <v>0</v>
       </c>
@@ -5414,7 +5408,7 @@
       <c r="BN22" s="7">
         <v>0</v>
       </c>
-      <c r="BO22" s="44"/>
+      <c r="BO22" s="35"/>
       <c r="BP22" s="7"/>
       <c r="CK22">
         <v>1</v>
@@ -5442,7 +5436,7 @@
       <c r="E23" s="1">
         <v>2</v>
       </c>
-      <c r="F23" s="44"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="8">
         <v>0</v>
       </c>
@@ -5458,8 +5452,8 @@
       <c r="K23" s="9">
         <v>0</v>
       </c>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
       <c r="N23" s="10">
         <v>0</v>
       </c>
@@ -5505,8 +5499,8 @@
       <c r="AB23" s="7">
         <v>0</v>
       </c>
-      <c r="AC23" s="44"/>
-      <c r="AD23" s="44"/>
+      <c r="AC23" s="35"/>
+      <c r="AD23" s="35"/>
       <c r="AE23" s="7">
         <v>0</v>
       </c>
@@ -5522,8 +5516,8 @@
       <c r="AI23" s="7">
         <v>0</v>
       </c>
-      <c r="AJ23" s="44"/>
-      <c r="AK23" s="44"/>
+      <c r="AJ23" s="35"/>
+      <c r="AK23" s="35"/>
       <c r="AL23" s="11">
         <v>0</v>
       </c>
@@ -5539,8 +5533,8 @@
       <c r="AP23" s="10">
         <v>0</v>
       </c>
-      <c r="AQ23" s="49"/>
-      <c r="AR23" s="49"/>
+      <c r="AQ23" s="40"/>
+      <c r="AR23" s="40"/>
       <c r="AS23" s="7">
         <v>0</v>
       </c>
@@ -5586,8 +5580,8 @@
       <c r="BG23" s="7">
         <v>0</v>
       </c>
-      <c r="BH23" s="44"/>
-      <c r="BI23" s="44"/>
+      <c r="BH23" s="35"/>
+      <c r="BI23" s="35"/>
       <c r="BJ23" s="7">
         <v>0</v>
       </c>
@@ -5603,7 +5597,7 @@
       <c r="BN23" s="7">
         <v>0</v>
       </c>
-      <c r="BO23" s="44"/>
+      <c r="BO23" s="35"/>
       <c r="BP23" s="7"/>
       <c r="CK23">
         <v>1</v>
@@ -5631,7 +5625,7 @@
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="44"/>
+      <c r="F24" s="35"/>
       <c r="G24" s="8">
         <v>1</v>
       </c>
@@ -5647,8 +5641,8 @@
       <c r="K24" s="9">
         <v>1</v>
       </c>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
       <c r="N24" s="10">
         <v>1</v>
       </c>
@@ -5694,8 +5688,8 @@
       <c r="AB24" s="7">
         <v>1</v>
       </c>
-      <c r="AC24" s="44"/>
-      <c r="AD24" s="44"/>
+      <c r="AC24" s="35"/>
+      <c r="AD24" s="35"/>
       <c r="AE24" s="7">
         <v>1</v>
       </c>
@@ -5711,8 +5705,8 @@
       <c r="AI24" s="7">
         <v>1</v>
       </c>
-      <c r="AJ24" s="44"/>
-      <c r="AK24" s="44"/>
+      <c r="AJ24" s="35"/>
+      <c r="AK24" s="35"/>
       <c r="AL24" s="11">
         <v>0</v>
       </c>
@@ -5728,8 +5722,8 @@
       <c r="AP24" s="10">
         <v>0</v>
       </c>
-      <c r="AQ24" s="49"/>
-      <c r="AR24" s="49"/>
+      <c r="AQ24" s="40"/>
+      <c r="AR24" s="40"/>
       <c r="AS24" s="7">
         <v>0</v>
       </c>
@@ -5775,8 +5769,8 @@
       <c r="BG24" s="7">
         <v>0</v>
       </c>
-      <c r="BH24" s="44"/>
-      <c r="BI24" s="44"/>
+      <c r="BH24" s="35"/>
+      <c r="BI24" s="35"/>
       <c r="BJ24" s="7">
         <v>0</v>
       </c>
@@ -5792,7 +5786,7 @@
       <c r="BN24" s="7">
         <v>0</v>
       </c>
-      <c r="BO24" s="44"/>
+      <c r="BO24" s="35"/>
       <c r="BP24" s="7"/>
       <c r="CU24" s="12">
         <v>73</v>
@@ -5817,7 +5811,7 @@
       <c r="E25" s="1">
         <v>2</v>
       </c>
-      <c r="F25" s="44"/>
+      <c r="F25" s="35"/>
       <c r="G25" s="8">
         <v>1</v>
       </c>
@@ -5833,8 +5827,8 @@
       <c r="K25" s="9">
         <v>1</v>
       </c>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
       <c r="N25" s="10">
         <v>1</v>
       </c>
@@ -5880,8 +5874,8 @@
       <c r="AB25" s="7">
         <v>1</v>
       </c>
-      <c r="AC25" s="44"/>
-      <c r="AD25" s="44"/>
+      <c r="AC25" s="35"/>
+      <c r="AD25" s="35"/>
       <c r="AE25" s="7">
         <v>1</v>
       </c>
@@ -5897,8 +5891,8 @@
       <c r="AI25" s="7">
         <v>1</v>
       </c>
-      <c r="AJ25" s="44"/>
-      <c r="AK25" s="44"/>
+      <c r="AJ25" s="35"/>
+      <c r="AK25" s="35"/>
       <c r="AL25" s="11">
         <v>0</v>
       </c>
@@ -5914,8 +5908,8 @@
       <c r="AP25" s="10">
         <v>0</v>
       </c>
-      <c r="AQ25" s="49"/>
-      <c r="AR25" s="49"/>
+      <c r="AQ25" s="40"/>
+      <c r="AR25" s="40"/>
       <c r="AS25" s="7">
         <v>0</v>
       </c>
@@ -5961,8 +5955,8 @@
       <c r="BG25" s="7">
         <v>0</v>
       </c>
-      <c r="BH25" s="44"/>
-      <c r="BI25" s="44"/>
+      <c r="BH25" s="35"/>
+      <c r="BI25" s="35"/>
       <c r="BJ25" s="7">
         <v>0</v>
       </c>
@@ -5978,7 +5972,7 @@
       <c r="BN25" s="7">
         <v>0</v>
       </c>
-      <c r="BO25" s="44"/>
+      <c r="BO25" s="35"/>
       <c r="BP25" s="7"/>
       <c r="CA25">
         <v>1</v>
@@ -6006,7 +6000,7 @@
       <c r="E26" s="1">
         <v>3</v>
       </c>
-      <c r="F26" s="44"/>
+      <c r="F26" s="35"/>
       <c r="G26" s="8">
         <v>1</v>
       </c>
@@ -6022,8 +6016,8 @@
       <c r="K26" s="9">
         <v>0</v>
       </c>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
       <c r="N26" s="10">
         <v>1</v>
       </c>
@@ -6069,8 +6063,8 @@
       <c r="AB26" s="7">
         <v>0</v>
       </c>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
+      <c r="AC26" s="35"/>
+      <c r="AD26" s="35"/>
       <c r="AE26" s="7">
         <v>1</v>
       </c>
@@ -6086,8 +6080,8 @@
       <c r="AI26" s="7">
         <v>0</v>
       </c>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
+      <c r="AJ26" s="35"/>
+      <c r="AK26" s="35"/>
       <c r="AL26" s="11">
         <v>0</v>
       </c>
@@ -6103,8 +6097,8 @@
       <c r="AP26" s="10">
         <v>0</v>
       </c>
-      <c r="AQ26" s="49"/>
-      <c r="AR26" s="49"/>
+      <c r="AQ26" s="40"/>
+      <c r="AR26" s="40"/>
       <c r="AS26" s="7">
         <v>0</v>
       </c>
@@ -6150,8 +6144,8 @@
       <c r="BG26" s="7">
         <v>0</v>
       </c>
-      <c r="BH26" s="44"/>
-      <c r="BI26" s="44"/>
+      <c r="BH26" s="35"/>
+      <c r="BI26" s="35"/>
       <c r="BJ26" s="7">
         <v>0</v>
       </c>
@@ -6167,7 +6161,7 @@
       <c r="BN26" s="7">
         <v>0</v>
       </c>
-      <c r="BO26" s="44"/>
+      <c r="BO26" s="35"/>
       <c r="BP26" s="7"/>
       <c r="CK26">
         <v>1</v>
@@ -6195,7 +6189,7 @@
       <c r="E27" s="1">
         <v>3</v>
       </c>
-      <c r="F27" s="44"/>
+      <c r="F27" s="35"/>
       <c r="G27" s="8">
         <v>0</v>
       </c>
@@ -6211,8 +6205,8 @@
       <c r="K27" s="9">
         <v>0</v>
       </c>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
       <c r="N27" s="10">
         <v>0</v>
       </c>
@@ -6258,8 +6252,8 @@
       <c r="AB27" s="7">
         <v>0</v>
       </c>
-      <c r="AC27" s="44"/>
-      <c r="AD27" s="44"/>
+      <c r="AC27" s="35"/>
+      <c r="AD27" s="35"/>
       <c r="AE27" s="7">
         <v>0</v>
       </c>
@@ -6275,8 +6269,8 @@
       <c r="AI27" s="7">
         <v>0</v>
       </c>
-      <c r="AJ27" s="44"/>
-      <c r="AK27" s="44"/>
+      <c r="AJ27" s="35"/>
+      <c r="AK27" s="35"/>
       <c r="AL27" s="11">
         <v>0</v>
       </c>
@@ -6292,8 +6286,8 @@
       <c r="AP27" s="10">
         <v>0</v>
       </c>
-      <c r="AQ27" s="49"/>
-      <c r="AR27" s="49"/>
+      <c r="AQ27" s="40"/>
+      <c r="AR27" s="40"/>
       <c r="AS27" s="7">
         <v>0</v>
       </c>
@@ -6339,8 +6333,8 @@
       <c r="BG27" s="7">
         <v>0</v>
       </c>
-      <c r="BH27" s="44"/>
-      <c r="BI27" s="44"/>
+      <c r="BH27" s="35"/>
+      <c r="BI27" s="35"/>
       <c r="BJ27" s="7">
         <v>0</v>
       </c>
@@ -6356,7 +6350,7 @@
       <c r="BN27" s="7">
         <v>0</v>
       </c>
-      <c r="BO27" s="44"/>
+      <c r="BO27" s="35"/>
       <c r="BP27" s="7"/>
       <c r="CK27">
         <v>1</v>
@@ -6384,7 +6378,7 @@
       <c r="E28" s="1">
         <v>1</v>
       </c>
-      <c r="F28" s="44"/>
+      <c r="F28" s="35"/>
       <c r="G28" s="8">
         <v>1</v>
       </c>
@@ -6400,8 +6394,8 @@
       <c r="K28" s="9">
         <v>1</v>
       </c>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
       <c r="N28" s="10">
         <v>0</v>
       </c>
@@ -6447,8 +6441,8 @@
       <c r="AB28" s="7">
         <v>0</v>
       </c>
-      <c r="AC28" s="44"/>
-      <c r="AD28" s="44"/>
+      <c r="AC28" s="35"/>
+      <c r="AD28" s="35"/>
       <c r="AE28" s="7">
         <v>1</v>
       </c>
@@ -6464,8 +6458,8 @@
       <c r="AI28" s="7">
         <v>1</v>
       </c>
-      <c r="AJ28" s="44"/>
-      <c r="AK28" s="44"/>
+      <c r="AJ28" s="35"/>
+      <c r="AK28" s="35"/>
       <c r="AL28" s="11">
         <v>1</v>
       </c>
@@ -6481,8 +6475,8 @@
       <c r="AP28" s="10">
         <v>0</v>
       </c>
-      <c r="AQ28" s="49"/>
-      <c r="AR28" s="49"/>
+      <c r="AQ28" s="40"/>
+      <c r="AR28" s="40"/>
       <c r="AS28" s="7">
         <v>1</v>
       </c>
@@ -6528,8 +6522,8 @@
       <c r="BG28" s="7">
         <v>0</v>
       </c>
-      <c r="BH28" s="44"/>
-      <c r="BI28" s="44"/>
+      <c r="BH28" s="35"/>
+      <c r="BI28" s="35"/>
       <c r="BJ28" s="7">
         <v>0</v>
       </c>
@@ -6545,7 +6539,7 @@
       <c r="BN28" s="7">
         <v>0</v>
       </c>
-      <c r="BO28" s="44"/>
+      <c r="BO28" s="35"/>
       <c r="BP28" s="7"/>
       <c r="CR28">
         <v>1</v>
@@ -6559,6 +6553,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="AS3:AU3"/>
+    <mergeCell ref="AV3:AX3"/>
+    <mergeCell ref="AY3:BA3"/>
+    <mergeCell ref="BB3:BD3"/>
+    <mergeCell ref="BE3:BG3"/>
     <mergeCell ref="BJ2:BN2"/>
     <mergeCell ref="AE2:AI2"/>
     <mergeCell ref="G1:AI1"/>
@@ -6567,16 +6571,6 @@
     <mergeCell ref="AS2:BG2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="N2:AB2"/>
-    <mergeCell ref="AS3:AU3"/>
-    <mergeCell ref="AV3:AX3"/>
-    <mergeCell ref="AY3:BA3"/>
-    <mergeCell ref="BB3:BD3"/>
-    <mergeCell ref="BE3:BG3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add crops to butterfly plants and plant location spreadsheets, which large and small white feed on
</commit_message>
<xml_diff>
--- a/Butterfly matrix.xlsx
+++ b/Butterfly matrix.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E3780F-B0EC-0C48-B80A-88705A196423}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8989B603-D379-C14E-B5AA-D1E201F72020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Species Set" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="2" r:id="rId2"/>
     <sheet name="larvae forage plants" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Full Species Set'!$A$1:$BQ$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,7 +51,7 @@
     <author>tc={33FF3A70-4CB3-A240-BDFC-FA10D8E6DB73}</author>
   </authors>
   <commentList>
-    <comment ref="CU4" authorId="0" shapeId="0" xr:uid="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
+    <comment ref="BP4" authorId="0" shapeId="0" xr:uid="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +59,7 @@
     This is Fa</t>
       </text>
     </comment>
-    <comment ref="CV4" authorId="1" shapeId="0" xr:uid="{100F15A9-7741-456F-AB72-27BB7A9AB780}">
+    <comment ref="BQ4" authorId="1" shapeId="0" xr:uid="{100F15A9-7741-456F-AB72-27BB7A9AB780}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -152,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="135">
   <si>
     <t>Species</t>
   </si>
@@ -521,99 +524,6 @@
   </si>
   <si>
     <t>L_R_damp</t>
-  </si>
-  <si>
-    <t>Aquifoliaceae</t>
-  </si>
-  <si>
-    <t>Araliaceae</t>
-  </si>
-  <si>
-    <t>Balsaminaceae</t>
-  </si>
-  <si>
-    <t>Boraginaceae</t>
-  </si>
-  <si>
-    <t>Campanulaceae</t>
-  </si>
-  <si>
-    <t>Cannabaceae</t>
-  </si>
-  <si>
-    <t>Caryophyllaceae</t>
-  </si>
-  <si>
-    <t>Compositae</t>
-  </si>
-  <si>
-    <t>Convolvulaceae</t>
-  </si>
-  <si>
-    <t>Cornaceae</t>
-  </si>
-  <si>
-    <t>Cruciferae</t>
-  </si>
-  <si>
-    <t>Dipsacaceae</t>
-  </si>
-  <si>
-    <t>Fabaceae</t>
-  </si>
-  <si>
-    <t>Grossulariaceae</t>
-  </si>
-  <si>
-    <t>Lamiaceae</t>
-  </si>
-  <si>
-    <t>Liliaceae</t>
-  </si>
-  <si>
-    <t>Lythraceae</t>
-  </si>
-  <si>
-    <t>Malvaceae</t>
-  </si>
-  <si>
-    <t>Onagraceae</t>
-  </si>
-  <si>
-    <t>Papaveraceae</t>
-  </si>
-  <si>
-    <t>Poaceae</t>
-  </si>
-  <si>
-    <t>Polygonaceae</t>
-  </si>
-  <si>
-    <t>Ranunculaceae</t>
-  </si>
-  <si>
-    <t>Rhamnaceae</t>
-  </si>
-  <si>
-    <t>Rosaceae</t>
-  </si>
-  <si>
-    <t>Salicaceae</t>
-  </si>
-  <si>
-    <t>Scrophulariaceae</t>
-  </si>
-  <si>
-    <t>Ulmaceae</t>
-  </si>
-  <si>
-    <t>Umbelliferae</t>
-  </si>
-  <si>
-    <t>Violaceae</t>
-  </si>
-  <si>
-    <t>Celastraceae</t>
   </si>
   <si>
     <t>Ad_hab_start</t>
@@ -656,7 +566,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,12 +583,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -820,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -901,16 +805,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1300,10 +1194,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="CU4" dT="2020-01-20T13:33:41.57" personId="{DC903E8D-CC64-4CAD-9C70-13197F8FDC74}" id="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
+  <threadedComment ref="BP4" dT="2020-01-20T13:33:41.57" personId="{DC903E8D-CC64-4CAD-9C70-13197F8FDC74}" id="{D46D3688-3EF9-40E7-80B0-6A21D710AA6A}">
     <text>This is Fa</text>
   </threadedComment>
-  <threadedComment ref="CV4" dT="2020-01-20T13:33:54.11" personId="{DC903E8D-CC64-4CAD-9C70-13197F8FDC74}" id="{100F15A9-7741-456F-AB72-27BB7A9AB780}">
+  <threadedComment ref="BQ4" dT="2020-01-20T13:33:54.11" personId="{DC903E8D-CC64-4CAD-9C70-13197F8FDC74}" id="{100F15A9-7741-456F-AB72-27BB7A9AB780}">
     <text>This is Fl</text>
   </threadedComment>
   <threadedComment ref="E8" dT="2021-04-15T18:05:37.40" personId="{415634E9-94E0-8F45-8A23-BD54341FBB2F}" id="{C66782A8-B31B-4B41-ABAC-0834AB6DC62E}">
@@ -1344,10 +1238,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CV28"/>
+  <dimension ref="A1:BQ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1356,13 +1251,13 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="30" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="9" max="9" width="9.83203125" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="34" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="30" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" customWidth="1"/>
     <col min="17" max="17" width="10.83203125" customWidth="1"/>
     <col min="18" max="19" width="9.83203125" customWidth="1"/>
@@ -1370,202 +1265,171 @@
     <col min="21" max="22" width="9.83203125" customWidth="1"/>
     <col min="23" max="23" width="10.6640625" customWidth="1"/>
     <col min="24" max="26" width="9.83203125" customWidth="1"/>
-    <col min="29" max="30" width="8.83203125" style="34"/>
+    <col min="29" max="30" width="8.83203125" style="30"/>
     <col min="31" max="31" width="10.5" customWidth="1"/>
     <col min="32" max="32" width="12.5" customWidth="1"/>
     <col min="33" max="33" width="12.83203125" customWidth="1"/>
     <col min="34" max="34" width="11.6640625" customWidth="1"/>
     <col min="35" max="35" width="12.6640625" customWidth="1"/>
-    <col min="36" max="36" width="9.5" style="34" customWidth="1"/>
-    <col min="37" max="37" width="9.1640625" style="34" customWidth="1"/>
+    <col min="36" max="36" width="9.5" style="30" customWidth="1"/>
+    <col min="37" max="37" width="9.1640625" style="30" customWidth="1"/>
     <col min="40" max="40" width="9.83203125" customWidth="1"/>
-    <col min="43" max="44" width="8.83203125" style="34"/>
+    <col min="43" max="44" width="8.83203125" style="30"/>
     <col min="51" max="51" width="9.83203125" customWidth="1"/>
     <col min="54" max="54" width="10.33203125" customWidth="1"/>
-    <col min="60" max="61" width="8.83203125" style="34"/>
+    <col min="60" max="61" width="8.83203125" style="30"/>
     <col min="63" max="63" width="10.5" customWidth="1"/>
     <col min="64" max="64" width="10.1640625" customWidth="1"/>
     <col min="65" max="65" width="11" customWidth="1"/>
     <col min="66" max="66" width="10.1640625" customWidth="1"/>
-    <col min="67" max="67" width="10.83203125" style="34" customWidth="1"/>
-    <col min="99" max="99" width="17.6640625" customWidth="1"/>
-    <col min="100" max="100" width="19.6640625" customWidth="1"/>
+    <col min="67" max="67" width="10.83203125" style="30" customWidth="1"/>
+    <col min="68" max="68" width="17.6640625" customWidth="1"/>
+    <col min="69" max="69" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="45" t="s">
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="AM1" s="45"/>
-      <c r="AN1" s="45"/>
-      <c r="AO1" s="45"/>
-      <c r="AP1" s="45"/>
-      <c r="AQ1" s="45"/>
-      <c r="AR1" s="45"/>
-      <c r="AS1" s="45"/>
-      <c r="AT1" s="45"/>
-      <c r="AU1" s="45"/>
-      <c r="AV1" s="45"/>
-      <c r="AW1" s="45"/>
-      <c r="AX1" s="45"/>
-      <c r="AY1" s="45"/>
-      <c r="AZ1" s="45"/>
-      <c r="BA1" s="45"/>
-      <c r="BB1" s="45"/>
-      <c r="BC1" s="45"/>
-      <c r="BD1" s="45"/>
-      <c r="BE1" s="45"/>
-      <c r="BF1" s="45"/>
-      <c r="BG1" s="45"/>
-      <c r="BH1" s="45"/>
-      <c r="BI1" s="45"/>
-      <c r="BJ1" s="45"/>
-      <c r="BK1" s="45"/>
-      <c r="BL1" s="45"/>
-      <c r="BM1" s="45"/>
-      <c r="BN1" s="45"/>
-      <c r="BO1" s="37"/>
-      <c r="BP1" s="33"/>
-      <c r="BQ1" s="33"/>
-      <c r="BR1" s="33"/>
-      <c r="BS1" s="33"/>
-      <c r="BT1" s="33"/>
-      <c r="BU1" s="33"/>
-      <c r="BV1" s="33"/>
-      <c r="BW1" s="33"/>
-      <c r="BX1" s="33"/>
-      <c r="BY1" s="33"/>
-      <c r="BZ1" s="33"/>
-      <c r="CA1" s="33"/>
-      <c r="CB1" s="33"/>
-      <c r="CC1" s="33"/>
-      <c r="CD1" s="33"/>
-      <c r="CE1" s="33"/>
-      <c r="CF1" s="33"/>
-      <c r="CG1" s="33"/>
-      <c r="CH1" s="33"/>
-      <c r="CI1" s="33"/>
-      <c r="CJ1" s="33"/>
-      <c r="CK1" s="33"/>
-      <c r="CL1" s="33"/>
-      <c r="CM1" s="33"/>
-      <c r="CN1" s="33"/>
-      <c r="CO1" s="33"/>
-      <c r="CP1" s="33"/>
-      <c r="CQ1" s="33"/>
-      <c r="CR1" s="33"/>
-      <c r="CS1" s="33"/>
-      <c r="CT1" s="33"/>
-    </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="G2" s="46" t="s">
+      <c r="AM1" s="41"/>
+      <c r="AN1" s="41"/>
+      <c r="AO1" s="41"/>
+      <c r="AP1" s="41"/>
+      <c r="AQ1" s="41"/>
+      <c r="AR1" s="41"/>
+      <c r="AS1" s="41"/>
+      <c r="AT1" s="41"/>
+      <c r="AU1" s="41"/>
+      <c r="AV1" s="41"/>
+      <c r="AW1" s="41"/>
+      <c r="AX1" s="41"/>
+      <c r="AY1" s="41"/>
+      <c r="AZ1" s="41"/>
+      <c r="BA1" s="41"/>
+      <c r="BB1" s="41"/>
+      <c r="BC1" s="41"/>
+      <c r="BD1" s="41"/>
+      <c r="BE1" s="41"/>
+      <c r="BF1" s="41"/>
+      <c r="BG1" s="41"/>
+      <c r="BH1" s="41"/>
+      <c r="BI1" s="41"/>
+      <c r="BJ1" s="41"/>
+      <c r="BK1" s="41"/>
+      <c r="BL1" s="41"/>
+      <c r="BM1" s="41"/>
+      <c r="BN1" s="41"/>
+      <c r="BO1" s="33"/>
+    </row>
+    <row r="2" spans="1:69" x14ac:dyDescent="0.2">
+      <c r="G2" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="N2" s="47" t="s">
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="N2" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="41" t="s">
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="AF2" s="42"/>
-      <c r="AG2" s="42"/>
-      <c r="AH2" s="42"/>
-      <c r="AI2" s="42"/>
-      <c r="AJ2" s="38"/>
-      <c r="AK2" s="38"/>
-      <c r="AL2" s="46" t="s">
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="37"/>
-      <c r="AR2" s="37"/>
-      <c r="AS2" s="47" t="s">
+      <c r="AM2" s="42"/>
+      <c r="AN2" s="42"/>
+      <c r="AO2" s="42"/>
+      <c r="AP2" s="42"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="AT2" s="47"/>
-      <c r="AU2" s="47"/>
-      <c r="AV2" s="47"/>
-      <c r="AW2" s="47"/>
-      <c r="AX2" s="47"/>
-      <c r="AY2" s="47"/>
-      <c r="AZ2" s="47"/>
-      <c r="BA2" s="47"/>
-      <c r="BB2" s="47"/>
-      <c r="BC2" s="47"/>
-      <c r="BD2" s="47"/>
-      <c r="BE2" s="47"/>
-      <c r="BF2" s="47"/>
-      <c r="BG2" s="47"/>
-      <c r="BH2" s="37"/>
-      <c r="BI2" s="37"/>
-      <c r="BJ2" s="41" t="s">
+      <c r="AT2" s="43"/>
+      <c r="AU2" s="43"/>
+      <c r="AV2" s="43"/>
+      <c r="AW2" s="43"/>
+      <c r="AX2" s="43"/>
+      <c r="AY2" s="43"/>
+      <c r="AZ2" s="43"/>
+      <c r="BA2" s="43"/>
+      <c r="BB2" s="43"/>
+      <c r="BC2" s="43"/>
+      <c r="BD2" s="43"/>
+      <c r="BE2" s="43"/>
+      <c r="BF2" s="43"/>
+      <c r="BG2" s="43"/>
+      <c r="BH2" s="33"/>
+      <c r="BI2" s="33"/>
+      <c r="BJ2" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="BK2" s="41"/>
-      <c r="BL2" s="41"/>
-      <c r="BM2" s="41"/>
-      <c r="BN2" s="41"/>
-      <c r="BO2" s="37"/>
-    </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.2">
+      <c r="BK2" s="37"/>
+      <c r="BL2" s="37"/>
+      <c r="BM2" s="37"/>
+      <c r="BN2" s="37"/>
+      <c r="BO2" s="33"/>
+    </row>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
       <c r="G3" s="14" t="s">
         <v>99</v>
       </c>
@@ -1581,33 +1445,33 @@
       <c r="K3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="49" t="s">
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="48" t="s">
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="U3" s="48"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="49" t="s">
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="48" t="s">
+      <c r="X3" s="45"/>
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="48"/>
-      <c r="AC3" s="38"/>
-      <c r="AD3" s="38"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="44"/>
+      <c r="AC3" s="34"/>
+      <c r="AD3" s="34"/>
       <c r="AE3" s="21" t="s">
         <v>99</v>
       </c>
@@ -1623,8 +1487,8 @@
       <c r="AI3" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="AJ3" s="38"/>
-      <c r="AK3" s="38"/>
+      <c r="AJ3" s="34"/>
+      <c r="AK3" s="34"/>
       <c r="AL3" s="14" t="s">
         <v>99</v>
       </c>
@@ -1640,35 +1504,35 @@
       <c r="AP3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="AQ3" s="38"/>
-      <c r="AR3" s="38"/>
-      <c r="AS3" s="48" t="s">
+      <c r="AQ3" s="34"/>
+      <c r="AR3" s="34"/>
+      <c r="AS3" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="AT3" s="48"/>
-      <c r="AU3" s="48"/>
-      <c r="AV3" s="49" t="s">
+      <c r="AT3" s="44"/>
+      <c r="AU3" s="44"/>
+      <c r="AV3" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="AW3" s="49"/>
-      <c r="AX3" s="49"/>
-      <c r="AY3" s="48" t="s">
+      <c r="AW3" s="45"/>
+      <c r="AX3" s="45"/>
+      <c r="AY3" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="AZ3" s="48"/>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="49" t="s">
+      <c r="AZ3" s="44"/>
+      <c r="BA3" s="44"/>
+      <c r="BB3" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="BC3" s="49"/>
-      <c r="BD3" s="49"/>
-      <c r="BE3" s="48" t="s">
+      <c r="BC3" s="45"/>
+      <c r="BD3" s="45"/>
+      <c r="BE3" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="38"/>
-      <c r="BI3" s="38"/>
+      <c r="BF3" s="44"/>
+      <c r="BG3" s="44"/>
+      <c r="BH3" s="34"/>
+      <c r="BI3" s="34"/>
       <c r="BJ3" s="21" t="s">
         <v>99</v>
       </c>
@@ -1684,9 +1548,9 @@
       <c r="BN3" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="BO3" s="38"/>
-    </row>
-    <row r="4" spans="1:100" ht="32" x14ac:dyDescent="0.2">
+      <c r="BO3" s="34"/>
+    </row>
+    <row r="4" spans="1:69" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1702,8 +1566,8 @@
       <c r="E4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="35" t="s">
-        <v>154</v>
+      <c r="F4" s="31" t="s">
+        <v>123</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>1</v>
@@ -1720,11 +1584,11 @@
       <c r="K4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="M4" s="36" t="s">
-        <v>156</v>
+      <c r="L4" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>125</v>
       </c>
       <c r="N4" s="19" t="s">
         <v>6</v>
@@ -1771,11 +1635,11 @@
       <c r="AB4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AC4" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="AD4" s="39" t="s">
-        <v>158</v>
+      <c r="AC4" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD4" s="35" t="s">
+        <v>127</v>
       </c>
       <c r="AE4" s="22" t="s">
         <v>113</v>
@@ -1792,11 +1656,11 @@
       <c r="AI4" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="AJ4" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="AK4" s="39" t="s">
-        <v>160</v>
+      <c r="AJ4" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK4" s="35" t="s">
+        <v>129</v>
       </c>
       <c r="AL4" s="25" t="s">
         <v>26</v>
@@ -1813,11 +1677,11 @@
       <c r="AP4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AQ4" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="AR4" s="39" t="s">
-        <v>162</v>
+      <c r="AQ4" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="AR4" s="35" t="s">
+        <v>131</v>
       </c>
       <c r="AS4" s="19" t="s">
         <v>31</v>
@@ -1864,11 +1728,11 @@
       <c r="BG4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="BH4" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="BI4" s="39" t="s">
-        <v>164</v>
+      <c r="BH4" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="BI4" s="35" t="s">
+        <v>133</v>
       </c>
       <c r="BJ4" s="22" t="s">
         <v>118</v>
@@ -1885,110 +1749,17 @@
       <c r="BN4" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="BO4" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="BP4" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="BQ4" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="BR4" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="BS4" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="BT4" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="BU4" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="BV4" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="BW4" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="BX4" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="BY4" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="BZ4" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="CA4" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="CB4" s="30" t="s">
+      <c r="BO4" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="CC4" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="CD4" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="CE4" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="CF4" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="CG4" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="CH4" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="CI4" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="CJ4" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="CK4" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="CL4" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="CM4" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="CN4" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="CO4" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="CP4" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="CQ4" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="CR4" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="CS4" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="CT4" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="CU4" s="6" t="s">
+      <c r="BP4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="CV4" s="5" t="s">
+      <c r="BQ4" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>48</v>
       </c>
@@ -2004,7 +1775,7 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="8">
         <v>1</v>
       </c>
@@ -2020,8 +1791,8 @@
       <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
       <c r="N5" s="10">
         <v>1</v>
       </c>
@@ -2067,8 +1838,8 @@
       <c r="AB5" s="7">
         <v>1</v>
       </c>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="35"/>
+      <c r="AC5" s="31"/>
+      <c r="AD5" s="31"/>
       <c r="AE5" s="7">
         <v>1</v>
       </c>
@@ -2084,8 +1855,8 @@
       <c r="AI5" s="7">
         <v>1</v>
       </c>
-      <c r="AJ5" s="35"/>
-      <c r="AK5" s="35"/>
+      <c r="AJ5" s="31"/>
+      <c r="AK5" s="31"/>
       <c r="AL5" s="11">
         <v>1</v>
       </c>
@@ -2101,8 +1872,8 @@
       <c r="AP5" s="10">
         <v>0</v>
       </c>
-      <c r="AQ5" s="40"/>
-      <c r="AR5" s="40"/>
+      <c r="AQ5" s="36"/>
+      <c r="AR5" s="36"/>
       <c r="AS5" s="7">
         <v>0</v>
       </c>
@@ -2148,8 +1919,8 @@
       <c r="BG5" s="7">
         <v>0</v>
       </c>
-      <c r="BH5" s="35"/>
-      <c r="BI5" s="35"/>
+      <c r="BH5" s="31"/>
+      <c r="BI5" s="31"/>
       <c r="BJ5" s="7">
         <v>1</v>
       </c>
@@ -2165,20 +1936,15 @@
       <c r="BN5" s="7">
         <v>0</v>
       </c>
-      <c r="BO5" s="35"/>
-      <c r="BQ5" s="30"/>
-      <c r="BR5" s="30"/>
-      <c r="CN5">
-        <v>1</v>
-      </c>
-      <c r="CU5" s="12">
+      <c r="BO5" s="31"/>
+      <c r="BP5" s="12">
         <v>73</v>
       </c>
-      <c r="CV5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.2">
+      <c r="BQ5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -2194,7 +1960,7 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="31"/>
       <c r="G6" s="8">
         <v>1</v>
       </c>
@@ -2210,8 +1976,8 @@
       <c r="K6" s="9">
         <v>0</v>
       </c>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
       <c r="N6" s="10">
         <v>0</v>
       </c>
@@ -2257,8 +2023,8 @@
       <c r="AB6" s="7">
         <v>0</v>
       </c>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
+      <c r="AC6" s="31"/>
+      <c r="AD6" s="31"/>
       <c r="AE6" s="7">
         <v>1</v>
       </c>
@@ -2274,8 +2040,8 @@
       <c r="AI6" s="7">
         <v>0</v>
       </c>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="35"/>
+      <c r="AJ6" s="31"/>
+      <c r="AK6" s="31"/>
       <c r="AL6" s="11">
         <v>1</v>
       </c>
@@ -2291,8 +2057,8 @@
       <c r="AP6" s="10">
         <v>0</v>
       </c>
-      <c r="AQ6" s="40"/>
-      <c r="AR6" s="40"/>
+      <c r="AQ6" s="36"/>
+      <c r="AR6" s="36"/>
       <c r="AS6" s="7">
         <v>1</v>
       </c>
@@ -2338,8 +2104,8 @@
       <c r="BG6" s="7">
         <v>0</v>
       </c>
-      <c r="BH6" s="35"/>
-      <c r="BI6" s="35"/>
+      <c r="BH6" s="31"/>
+      <c r="BI6" s="31"/>
       <c r="BJ6" s="7">
         <v>0</v>
       </c>
@@ -2355,21 +2121,15 @@
       <c r="BN6" s="7">
         <v>0</v>
       </c>
-      <c r="BO6" s="35"/>
-      <c r="BQ6" s="31"/>
-      <c r="BR6" s="31"/>
-      <c r="CN6" s="32"/>
-      <c r="CO6">
-        <v>1</v>
-      </c>
-      <c r="CU6" s="13">
+      <c r="BO6" s="31"/>
+      <c r="BP6" s="13">
         <v>27</v>
       </c>
-      <c r="CV6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.2">
+      <c r="BQ6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>50</v>
       </c>
@@ -2385,7 +2145,7 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="31"/>
       <c r="G7" s="8">
         <v>1</v>
       </c>
@@ -2401,8 +2161,8 @@
       <c r="K7" s="9">
         <v>1</v>
       </c>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
       <c r="N7" s="10">
         <v>1</v>
       </c>
@@ -2448,8 +2208,8 @@
       <c r="AB7" s="7">
         <v>1</v>
       </c>
-      <c r="AC7" s="35"/>
-      <c r="AD7" s="35"/>
+      <c r="AC7" s="31"/>
+      <c r="AD7" s="31"/>
       <c r="AE7" s="7">
         <v>1</v>
       </c>
@@ -2465,8 +2225,8 @@
       <c r="AI7" s="7">
         <v>1</v>
       </c>
-      <c r="AJ7" s="35"/>
-      <c r="AK7" s="35"/>
+      <c r="AJ7" s="31"/>
+      <c r="AK7" s="31"/>
       <c r="AL7" s="11">
         <v>1</v>
       </c>
@@ -2482,8 +2242,8 @@
       <c r="AP7" s="10">
         <v>0</v>
       </c>
-      <c r="AQ7" s="40"/>
-      <c r="AR7" s="40"/>
+      <c r="AQ7" s="36"/>
+      <c r="AR7" s="36"/>
       <c r="AS7" s="7">
         <v>1</v>
       </c>
@@ -2529,8 +2289,8 @@
       <c r="BG7" s="7">
         <v>0</v>
       </c>
-      <c r="BH7" s="35"/>
-      <c r="BI7" s="35"/>
+      <c r="BH7" s="31"/>
+      <c r="BI7" s="31"/>
       <c r="BJ7" s="7">
         <v>1</v>
       </c>
@@ -2546,28 +2306,15 @@
       <c r="BN7" s="7">
         <v>0</v>
       </c>
-      <c r="BO7" s="35"/>
-      <c r="BP7" s="7"/>
-      <c r="BU7">
-        <v>1</v>
-      </c>
-      <c r="CD7">
-        <v>1</v>
-      </c>
-      <c r="CP7">
-        <v>1</v>
-      </c>
-      <c r="CR7">
-        <v>1</v>
-      </c>
-      <c r="CU7" s="12">
+      <c r="BO7" s="31"/>
+      <c r="BP7" s="12">
         <v>73</v>
       </c>
-      <c r="CV7" s="7">
+      <c r="BQ7" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>51</v>
       </c>
@@ -2583,7 +2330,7 @@
       <c r="E8" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="35"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="8">
         <v>1</v>
       </c>
@@ -2599,8 +2346,8 @@
       <c r="K8" s="9">
         <v>0</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
       <c r="N8" s="10">
         <v>1</v>
       </c>
@@ -2646,8 +2393,8 @@
       <c r="AB8" s="7">
         <v>0</v>
       </c>
-      <c r="AC8" s="35"/>
-      <c r="AD8" s="35"/>
+      <c r="AC8" s="31"/>
+      <c r="AD8" s="31"/>
       <c r="AE8" s="7">
         <v>1</v>
       </c>
@@ -2663,8 +2410,8 @@
       <c r="AI8" s="7">
         <v>0</v>
       </c>
-      <c r="AJ8" s="35"/>
-      <c r="AK8" s="35"/>
+      <c r="AJ8" s="31"/>
+      <c r="AK8" s="31"/>
       <c r="AL8" s="11">
         <v>0</v>
       </c>
@@ -2680,8 +2427,8 @@
       <c r="AP8" s="10">
         <v>0</v>
       </c>
-      <c r="AQ8" s="40"/>
-      <c r="AR8" s="40"/>
+      <c r="AQ8" s="36"/>
+      <c r="AR8" s="36"/>
       <c r="AS8" s="7">
         <v>0</v>
       </c>
@@ -2727,8 +2474,8 @@
       <c r="BG8" s="7">
         <v>0</v>
       </c>
-      <c r="BH8" s="35"/>
-      <c r="BI8" s="35"/>
+      <c r="BH8" s="31"/>
+      <c r="BI8" s="31"/>
       <c r="BJ8" s="7">
         <v>0</v>
       </c>
@@ -2744,19 +2491,15 @@
       <c r="BN8" s="7">
         <v>0</v>
       </c>
-      <c r="BO8" s="35"/>
-      <c r="BP8" s="7"/>
-      <c r="CC8">
-        <v>1</v>
-      </c>
-      <c r="CU8" s="12">
+      <c r="BO8" s="31"/>
+      <c r="BP8" s="12">
         <v>59</v>
       </c>
-      <c r="CV8" s="1">
+      <c r="BQ8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>52</v>
       </c>
@@ -2772,7 +2515,7 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" s="35"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="8">
         <v>0</v>
       </c>
@@ -2788,8 +2531,8 @@
       <c r="K9" s="9">
         <v>0</v>
       </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
       <c r="N9" s="10">
         <v>0</v>
       </c>
@@ -2835,8 +2578,8 @@
       <c r="AB9" s="7">
         <v>0</v>
       </c>
-      <c r="AC9" s="35"/>
-      <c r="AD9" s="35"/>
+      <c r="AC9" s="31"/>
+      <c r="AD9" s="31"/>
       <c r="AE9" s="7">
         <v>0</v>
       </c>
@@ -2852,8 +2595,8 @@
       <c r="AI9" s="7">
         <v>0</v>
       </c>
-      <c r="AJ9" s="35"/>
-      <c r="AK9" s="35"/>
+      <c r="AJ9" s="31"/>
+      <c r="AK9" s="31"/>
       <c r="AL9" s="11">
         <v>0</v>
       </c>
@@ -2869,8 +2612,8 @@
       <c r="AP9" s="10">
         <v>0</v>
       </c>
-      <c r="AQ9" s="40"/>
-      <c r="AR9" s="40"/>
+      <c r="AQ9" s="36"/>
+      <c r="AR9" s="36"/>
       <c r="AS9" s="7">
         <v>0</v>
       </c>
@@ -2916,8 +2659,8 @@
       <c r="BG9" s="7">
         <v>0</v>
       </c>
-      <c r="BH9" s="35"/>
-      <c r="BI9" s="35"/>
+      <c r="BH9" s="31"/>
+      <c r="BI9" s="31"/>
       <c r="BJ9" s="7">
         <v>0</v>
       </c>
@@ -2933,20 +2676,15 @@
       <c r="BN9" s="7">
         <v>0</v>
       </c>
-      <c r="BO9" s="35"/>
-      <c r="BP9" s="7"/>
-      <c r="BV9" s="30"/>
-      <c r="CK9">
-        <v>1</v>
-      </c>
-      <c r="CU9" s="12">
+      <c r="BO9" s="31"/>
+      <c r="BP9" s="12">
         <v>29</v>
       </c>
-      <c r="CV9" s="1">
+      <c r="BQ9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>53</v>
       </c>
@@ -2962,7 +2700,7 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="F10" s="35"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="8">
         <v>1</v>
       </c>
@@ -2978,8 +2716,8 @@
       <c r="K10" s="9">
         <v>0</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
       <c r="N10" s="10">
         <v>0</v>
       </c>
@@ -3025,8 +2763,8 @@
       <c r="AB10" s="7">
         <v>0</v>
       </c>
-      <c r="AC10" s="35"/>
-      <c r="AD10" s="35"/>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
       <c r="AE10" s="7">
         <v>1</v>
       </c>
@@ -3042,8 +2780,8 @@
       <c r="AI10" s="7">
         <v>0</v>
       </c>
-      <c r="AJ10" s="35"/>
-      <c r="AK10" s="35"/>
+      <c r="AJ10" s="31"/>
+      <c r="AK10" s="31"/>
       <c r="AL10" s="11">
         <v>0</v>
       </c>
@@ -3059,8 +2797,8 @@
       <c r="AP10" s="10">
         <v>0</v>
       </c>
-      <c r="AQ10" s="40"/>
-      <c r="AR10" s="40"/>
+      <c r="AQ10" s="36"/>
+      <c r="AR10" s="36"/>
       <c r="AS10" s="7">
         <v>0</v>
       </c>
@@ -3106,8 +2844,8 @@
       <c r="BG10" s="7">
         <v>0</v>
       </c>
-      <c r="BH10" s="35"/>
-      <c r="BI10" s="35"/>
+      <c r="BH10" s="31"/>
+      <c r="BI10" s="31"/>
       <c r="BJ10" s="7">
         <v>0</v>
       </c>
@@ -3123,19 +2861,15 @@
       <c r="BN10" s="7">
         <v>0</v>
       </c>
-      <c r="BO10" s="35"/>
-      <c r="BP10" s="7"/>
-      <c r="CK10">
-        <v>1</v>
-      </c>
-      <c r="CU10" s="12">
+      <c r="BO10" s="31"/>
+      <c r="BP10" s="12">
         <v>41</v>
       </c>
-      <c r="CV10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.2">
+      <c r="BQ10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -3151,7 +2885,7 @@
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="35"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="8">
         <v>1</v>
       </c>
@@ -3167,8 +2901,8 @@
       <c r="K11" s="9">
         <v>1</v>
       </c>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
       <c r="N11" s="10">
         <v>1</v>
       </c>
@@ -3214,8 +2948,8 @@
       <c r="AB11" s="7">
         <v>1</v>
       </c>
-      <c r="AC11" s="35"/>
-      <c r="AD11" s="35"/>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="31"/>
       <c r="AE11" s="7">
         <v>1</v>
       </c>
@@ -3231,8 +2965,8 @@
       <c r="AI11" s="7">
         <v>1</v>
       </c>
-      <c r="AJ11" s="35"/>
-      <c r="AK11" s="35"/>
+      <c r="AJ11" s="31"/>
+      <c r="AK11" s="31"/>
       <c r="AL11" s="11">
         <v>0</v>
       </c>
@@ -3248,8 +2982,8 @@
       <c r="AP11" s="10">
         <v>0</v>
       </c>
-      <c r="AQ11" s="40"/>
-      <c r="AR11" s="40"/>
+      <c r="AQ11" s="36"/>
+      <c r="AR11" s="36"/>
       <c r="AS11" s="7">
         <v>0</v>
       </c>
@@ -3295,8 +3029,8 @@
       <c r="BG11" s="7">
         <v>0</v>
       </c>
-      <c r="BH11" s="35"/>
-      <c r="BI11" s="35"/>
+      <c r="BH11" s="31"/>
+      <c r="BI11" s="31"/>
       <c r="BJ11" s="7">
         <v>0</v>
       </c>
@@ -3312,19 +3046,15 @@
       <c r="BN11" s="7">
         <v>0</v>
       </c>
-      <c r="BO11" s="35"/>
-      <c r="BP11" s="7"/>
-      <c r="CA11">
-        <v>1</v>
-      </c>
-      <c r="CU11" s="12">
+      <c r="BO11" s="31"/>
+      <c r="BP11" s="12">
         <v>73</v>
       </c>
-      <c r="CV11" s="1">
+      <c r="BQ11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
@@ -3340,7 +3070,7 @@
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" s="35"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="8">
         <v>1</v>
       </c>
@@ -3356,8 +3086,8 @@
       <c r="K12" s="9">
         <v>0</v>
       </c>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
       <c r="N12" s="10">
         <v>1</v>
       </c>
@@ -3403,8 +3133,8 @@
       <c r="AB12" s="7">
         <v>0</v>
       </c>
-      <c r="AC12" s="35"/>
-      <c r="AD12" s="35"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
       <c r="AE12" s="7">
         <v>1</v>
       </c>
@@ -3420,8 +3150,8 @@
       <c r="AI12" s="7">
         <v>0</v>
       </c>
-      <c r="AJ12" s="35"/>
-      <c r="AK12" s="35"/>
+      <c r="AJ12" s="31"/>
+      <c r="AK12" s="31"/>
       <c r="AL12" s="11">
         <v>1</v>
       </c>
@@ -3437,8 +3167,8 @@
       <c r="AP12" s="10">
         <v>0</v>
       </c>
-      <c r="AQ12" s="40"/>
-      <c r="AR12" s="40"/>
+      <c r="AQ12" s="36"/>
+      <c r="AR12" s="36"/>
       <c r="AS12" s="7">
         <v>1</v>
       </c>
@@ -3484,8 +3214,8 @@
       <c r="BG12" s="7">
         <v>0</v>
       </c>
-      <c r="BH12" s="35"/>
-      <c r="BI12" s="35"/>
+      <c r="BH12" s="31"/>
+      <c r="BI12" s="31"/>
       <c r="BJ12" s="7">
         <v>0</v>
       </c>
@@ -3501,36 +3231,15 @@
       <c r="BN12" s="7">
         <v>0</v>
       </c>
-      <c r="BO12" s="35"/>
-      <c r="BP12" s="1">
-        <v>1</v>
+      <c r="BO12" s="31"/>
+      <c r="BP12" s="12">
+        <v>59</v>
       </c>
       <c r="BQ12" s="1">
-        <v>1</v>
-      </c>
-      <c r="BW12">
-        <v>1</v>
-      </c>
-      <c r="BZ12">
-        <v>1</v>
-      </c>
-      <c r="CC12">
-        <v>1</v>
-      </c>
-      <c r="CN12">
-        <v>1</v>
-      </c>
-      <c r="CO12">
-        <v>1</v>
-      </c>
-      <c r="CU12" s="12">
-        <v>59</v>
-      </c>
-      <c r="CV12" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
@@ -3546,7 +3255,7 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="35"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="8">
         <v>0</v>
       </c>
@@ -3562,8 +3271,8 @@
       <c r="K13" s="9">
         <v>0</v>
       </c>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
       <c r="N13" s="10">
         <v>0</v>
       </c>
@@ -3609,8 +3318,8 @@
       <c r="AB13" s="7">
         <v>0</v>
       </c>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="31"/>
       <c r="AE13" s="7">
         <v>0</v>
       </c>
@@ -3626,8 +3335,8 @@
       <c r="AI13" s="7">
         <v>0</v>
       </c>
-      <c r="AJ13" s="35"/>
-      <c r="AK13" s="35"/>
+      <c r="AJ13" s="31"/>
+      <c r="AK13" s="31"/>
       <c r="AL13" s="11">
         <v>0</v>
       </c>
@@ -3643,8 +3352,8 @@
       <c r="AP13" s="10">
         <v>0</v>
       </c>
-      <c r="AQ13" s="40"/>
-      <c r="AR13" s="40"/>
+      <c r="AQ13" s="36"/>
+      <c r="AR13" s="36"/>
       <c r="AS13" s="7">
         <v>0</v>
       </c>
@@ -3690,8 +3399,8 @@
       <c r="BG13" s="7">
         <v>0</v>
       </c>
-      <c r="BH13" s="35"/>
-      <c r="BI13" s="35"/>
+      <c r="BH13" s="31"/>
+      <c r="BI13" s="31"/>
       <c r="BJ13" s="7">
         <v>0</v>
       </c>
@@ -3707,19 +3416,15 @@
       <c r="BN13" s="7">
         <v>0</v>
       </c>
-      <c r="BO13" s="35"/>
-      <c r="BP13" s="7"/>
-      <c r="CK13">
-        <v>1</v>
-      </c>
-      <c r="CU13" s="12">
+      <c r="BO13" s="31"/>
+      <c r="BP13" s="12">
         <v>29</v>
       </c>
-      <c r="CV13" s="1">
+      <c r="BQ13" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>57</v>
       </c>
@@ -3735,7 +3440,7 @@
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="35"/>
+      <c r="F14" s="31"/>
       <c r="G14" s="8">
         <v>1</v>
       </c>
@@ -3751,8 +3456,8 @@
       <c r="K14" s="9">
         <v>1</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
       <c r="N14" s="10">
         <v>1</v>
       </c>
@@ -3798,8 +3503,8 @@
       <c r="AB14" s="7">
         <v>1</v>
       </c>
-      <c r="AC14" s="35"/>
-      <c r="AD14" s="35"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
       <c r="AE14" s="7">
         <v>1</v>
       </c>
@@ -3815,8 +3520,8 @@
       <c r="AI14" s="7">
         <v>1</v>
       </c>
-      <c r="AJ14" s="35"/>
-      <c r="AK14" s="35"/>
+      <c r="AJ14" s="31"/>
+      <c r="AK14" s="31"/>
       <c r="AL14" s="11">
         <v>0</v>
       </c>
@@ -3832,8 +3537,8 @@
       <c r="AP14" s="10">
         <v>0</v>
       </c>
-      <c r="AQ14" s="40"/>
-      <c r="AR14" s="40"/>
+      <c r="AQ14" s="36"/>
+      <c r="AR14" s="36"/>
       <c r="AS14" s="7">
         <v>0</v>
       </c>
@@ -3879,8 +3584,8 @@
       <c r="BG14" s="7">
         <v>0</v>
       </c>
-      <c r="BH14" s="35"/>
-      <c r="BI14" s="35"/>
+      <c r="BH14" s="31"/>
+      <c r="BI14" s="31"/>
       <c r="BJ14" s="7">
         <v>0</v>
       </c>
@@ -3896,19 +3601,15 @@
       <c r="BN14" s="7">
         <v>0</v>
       </c>
-      <c r="BO14" s="35"/>
-      <c r="BP14" s="7"/>
-      <c r="CA14">
-        <v>1</v>
-      </c>
-      <c r="CU14" s="12">
+      <c r="BO14" s="31"/>
+      <c r="BP14" s="12">
         <v>73</v>
       </c>
-      <c r="CV14" s="1">
+      <c r="BQ14" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>58</v>
       </c>
@@ -3924,7 +3625,7 @@
       <c r="E15" s="1">
         <v>2</v>
       </c>
-      <c r="F15" s="35"/>
+      <c r="F15" s="31"/>
       <c r="G15" s="8">
         <v>1</v>
       </c>
@@ -3940,8 +3641,8 @@
       <c r="K15" s="9">
         <v>0</v>
       </c>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="10">
         <v>0</v>
       </c>
@@ -3987,8 +3688,8 @@
       <c r="AB15" s="7">
         <v>0</v>
       </c>
-      <c r="AC15" s="35"/>
-      <c r="AD15" s="35"/>
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="31"/>
       <c r="AE15" s="7">
         <v>1</v>
       </c>
@@ -4004,8 +3705,8 @@
       <c r="AI15" s="7">
         <v>0</v>
       </c>
-      <c r="AJ15" s="35"/>
-      <c r="AK15" s="35"/>
+      <c r="AJ15" s="31"/>
+      <c r="AK15" s="31"/>
       <c r="AL15" s="11">
         <v>0</v>
       </c>
@@ -4021,8 +3722,8 @@
       <c r="AP15" s="10">
         <v>0</v>
       </c>
-      <c r="AQ15" s="40"/>
-      <c r="AR15" s="40"/>
+      <c r="AQ15" s="36"/>
+      <c r="AR15" s="36"/>
       <c r="AS15" s="7">
         <v>0</v>
       </c>
@@ -4068,8 +3769,8 @@
       <c r="BG15" s="7">
         <v>0</v>
       </c>
-      <c r="BH15" s="35"/>
-      <c r="BI15" s="35"/>
+      <c r="BH15" s="31"/>
+      <c r="BI15" s="31"/>
       <c r="BJ15" s="7">
         <v>0</v>
       </c>
@@ -4085,19 +3786,15 @@
       <c r="BN15" s="7">
         <v>0</v>
       </c>
-      <c r="BO15" s="35"/>
-      <c r="BP15" s="7"/>
-      <c r="CK15">
-        <v>1</v>
-      </c>
-      <c r="CU15" s="12">
+      <c r="BO15" s="31"/>
+      <c r="BP15" s="12">
         <v>56</v>
       </c>
-      <c r="CV15" s="1">
+      <c r="BQ15" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>59</v>
       </c>
@@ -4113,7 +3810,7 @@
       <c r="E16" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="35"/>
+      <c r="F16" s="31"/>
       <c r="G16" s="8">
         <v>0</v>
       </c>
@@ -4129,8 +3826,8 @@
       <c r="K16" s="9">
         <v>0</v>
       </c>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
       <c r="N16" s="10">
         <v>0</v>
       </c>
@@ -4176,8 +3873,8 @@
       <c r="AB16" s="7">
         <v>0</v>
       </c>
-      <c r="AC16" s="35"/>
-      <c r="AD16" s="35"/>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="31"/>
       <c r="AE16" s="7">
         <v>0</v>
       </c>
@@ -4193,8 +3890,8 @@
       <c r="AI16" s="7">
         <v>0</v>
       </c>
-      <c r="AJ16" s="35"/>
-      <c r="AK16" s="35"/>
+      <c r="AJ16" s="31"/>
+      <c r="AK16" s="31"/>
       <c r="AL16" s="11">
         <v>0</v>
       </c>
@@ -4210,8 +3907,8 @@
       <c r="AP16" s="10">
         <v>0</v>
       </c>
-      <c r="AQ16" s="40"/>
-      <c r="AR16" s="40"/>
+      <c r="AQ16" s="36"/>
+      <c r="AR16" s="36"/>
       <c r="AS16" s="7">
         <v>0</v>
       </c>
@@ -4257,8 +3954,8 @@
       <c r="BG16" s="7">
         <v>0</v>
       </c>
-      <c r="BH16" s="35"/>
-      <c r="BI16" s="35"/>
+      <c r="BH16" s="31"/>
+      <c r="BI16" s="31"/>
       <c r="BJ16" s="7">
         <v>0</v>
       </c>
@@ -4274,19 +3971,15 @@
       <c r="BN16" s="7">
         <v>0</v>
       </c>
-      <c r="BO16" s="35"/>
-      <c r="BP16" s="7"/>
-      <c r="CB16">
-        <v>1</v>
-      </c>
-      <c r="CU16" s="12">
+      <c r="BO16" s="31"/>
+      <c r="BP16" s="12">
         <v>15</v>
       </c>
-      <c r="CV16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:100" x14ac:dyDescent="0.2">
+      <c r="BQ16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>60</v>
       </c>
@@ -4302,7 +3995,7 @@
       <c r="E17" s="1">
         <v>2</v>
       </c>
-      <c r="F17" s="35"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="8">
         <v>1</v>
       </c>
@@ -4318,8 +4011,8 @@
       <c r="K17" s="9">
         <v>0</v>
       </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
       <c r="N17" s="10">
         <v>0</v>
       </c>
@@ -4365,8 +4058,8 @@
       <c r="AB17" s="7">
         <v>0</v>
       </c>
-      <c r="AC17" s="35"/>
-      <c r="AD17" s="35"/>
+      <c r="AC17" s="31"/>
+      <c r="AD17" s="31"/>
       <c r="AE17" s="7">
         <v>1</v>
       </c>
@@ -4382,8 +4075,8 @@
       <c r="AI17" s="7">
         <v>0</v>
       </c>
-      <c r="AJ17" s="35"/>
-      <c r="AK17" s="35"/>
+      <c r="AJ17" s="31"/>
+      <c r="AK17" s="31"/>
       <c r="AL17" s="11">
         <v>0</v>
       </c>
@@ -4399,8 +4092,8 @@
       <c r="AP17" s="10">
         <v>0</v>
       </c>
-      <c r="AQ17" s="40"/>
-      <c r="AR17" s="40"/>
+      <c r="AQ17" s="36"/>
+      <c r="AR17" s="36"/>
       <c r="AS17" s="7">
         <v>0</v>
       </c>
@@ -4446,8 +4139,8 @@
       <c r="BG17" s="7">
         <v>0</v>
       </c>
-      <c r="BH17" s="35"/>
-      <c r="BI17" s="35"/>
+      <c r="BH17" s="31"/>
+      <c r="BI17" s="31"/>
       <c r="BJ17" s="7">
         <v>0</v>
       </c>
@@ -4463,19 +4156,15 @@
       <c r="BN17" s="7">
         <v>0</v>
       </c>
-      <c r="BO17" s="35"/>
-      <c r="BP17" s="7"/>
-      <c r="CK17">
-        <v>1</v>
-      </c>
-      <c r="CU17" s="12">
+      <c r="BO17" s="31"/>
+      <c r="BP17" s="12">
         <v>59</v>
       </c>
-      <c r="CV17" s="1">
+      <c r="BQ17" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>61</v>
       </c>
@@ -4491,7 +4180,7 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="35"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="8">
         <v>1</v>
       </c>
@@ -4507,8 +4196,8 @@
       <c r="K18" s="9">
         <v>1</v>
       </c>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
       <c r="N18" s="10">
         <v>1</v>
       </c>
@@ -4554,8 +4243,8 @@
       <c r="AB18" s="7">
         <v>0</v>
       </c>
-      <c r="AC18" s="35"/>
-      <c r="AD18" s="35"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31"/>
       <c r="AE18" s="7">
         <v>1</v>
       </c>
@@ -4571,8 +4260,8 @@
       <c r="AI18" s="7">
         <v>1</v>
       </c>
-      <c r="AJ18" s="35"/>
-      <c r="AK18" s="35"/>
+      <c r="AJ18" s="31"/>
+      <c r="AK18" s="31"/>
       <c r="AL18" s="11">
         <v>0</v>
       </c>
@@ -4588,8 +4277,8 @@
       <c r="AP18" s="10">
         <v>1</v>
       </c>
-      <c r="AQ18" s="40"/>
-      <c r="AR18" s="40"/>
+      <c r="AQ18" s="36"/>
+      <c r="AR18" s="36"/>
       <c r="AS18" s="7">
         <v>0</v>
       </c>
@@ -4635,8 +4324,8 @@
       <c r="BG18" s="7">
         <v>0</v>
       </c>
-      <c r="BH18" s="35"/>
-      <c r="BI18" s="35"/>
+      <c r="BH18" s="31"/>
+      <c r="BI18" s="31"/>
       <c r="BJ18" s="7">
         <v>0</v>
       </c>
@@ -4652,19 +4341,15 @@
       <c r="BN18" s="7">
         <v>0</v>
       </c>
-      <c r="BO18" s="35"/>
-      <c r="BP18" s="7"/>
-      <c r="CA18">
-        <v>1</v>
-      </c>
-      <c r="CU18" s="12">
+      <c r="BO18" s="31"/>
+      <c r="BP18" s="12">
         <v>73</v>
       </c>
-      <c r="CV18" s="1">
+      <c r="BQ18" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>62</v>
       </c>
@@ -4680,7 +4365,7 @@
       <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="35"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="8">
         <v>1</v>
       </c>
@@ -4696,8 +4381,8 @@
       <c r="K19" s="9">
         <v>1</v>
       </c>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
       <c r="N19" s="10">
         <v>1</v>
       </c>
@@ -4743,8 +4428,8 @@
       <c r="AB19" s="7">
         <v>1</v>
       </c>
-      <c r="AC19" s="35"/>
-      <c r="AD19" s="35"/>
+      <c r="AC19" s="31"/>
+      <c r="AD19" s="31"/>
       <c r="AE19" s="7">
         <v>1</v>
       </c>
@@ -4760,8 +4445,8 @@
       <c r="AI19" s="7">
         <v>1</v>
       </c>
-      <c r="AJ19" s="35"/>
-      <c r="AK19" s="35"/>
+      <c r="AJ19" s="31"/>
+      <c r="AK19" s="31"/>
       <c r="AL19" s="11">
         <v>0</v>
       </c>
@@ -4777,8 +4462,8 @@
       <c r="AP19" s="10">
         <v>0</v>
       </c>
-      <c r="AQ19" s="40"/>
-      <c r="AR19" s="40"/>
+      <c r="AQ19" s="36"/>
+      <c r="AR19" s="36"/>
       <c r="AS19" s="7">
         <v>0</v>
       </c>
@@ -4824,8 +4509,8 @@
       <c r="BG19" s="7">
         <v>0</v>
       </c>
-      <c r="BH19" s="35"/>
-      <c r="BI19" s="35"/>
+      <c r="BH19" s="31"/>
+      <c r="BI19" s="31"/>
       <c r="BJ19" s="7">
         <v>0</v>
       </c>
@@ -4841,19 +4526,15 @@
       <c r="BN19" s="7">
         <v>0</v>
       </c>
-      <c r="BO19" s="35"/>
-      <c r="BP19" s="7"/>
-      <c r="BU19">
-        <v>1</v>
-      </c>
-      <c r="CU19" s="12">
+      <c r="BO19" s="31"/>
+      <c r="BP19" s="12">
         <v>73</v>
       </c>
-      <c r="CV19" s="1">
+      <c r="BQ19" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>63</v>
       </c>
@@ -4869,7 +4550,7 @@
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="35"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="8">
         <v>1</v>
       </c>
@@ -4885,8 +4566,8 @@
       <c r="K20" s="9">
         <v>1</v>
       </c>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
       <c r="N20" s="10">
         <v>0</v>
       </c>
@@ -4932,8 +4613,8 @@
       <c r="AB20" s="7">
         <v>0</v>
       </c>
-      <c r="AC20" s="35"/>
-      <c r="AD20" s="35"/>
+      <c r="AC20" s="31"/>
+      <c r="AD20" s="31"/>
       <c r="AE20" s="7">
         <v>1</v>
       </c>
@@ -4949,8 +4630,8 @@
       <c r="AI20" s="7">
         <v>1</v>
       </c>
-      <c r="AJ20" s="35"/>
-      <c r="AK20" s="35"/>
+      <c r="AJ20" s="31"/>
+      <c r="AK20" s="31"/>
       <c r="AL20" s="11">
         <v>0</v>
       </c>
@@ -4966,8 +4647,8 @@
       <c r="AP20" s="10">
         <v>1</v>
       </c>
-      <c r="AQ20" s="40"/>
-      <c r="AR20" s="40"/>
+      <c r="AQ20" s="36"/>
+      <c r="AR20" s="36"/>
       <c r="AS20" s="7">
         <v>0</v>
       </c>
@@ -5013,8 +4694,8 @@
       <c r="BG20" s="7">
         <v>0</v>
       </c>
-      <c r="BH20" s="35"/>
-      <c r="BI20" s="35"/>
+      <c r="BH20" s="31"/>
+      <c r="BI20" s="31"/>
       <c r="BJ20" s="7">
         <v>0</v>
       </c>
@@ -5030,19 +4711,15 @@
       <c r="BN20" s="7">
         <v>0</v>
       </c>
-      <c r="BO20" s="35"/>
-      <c r="BP20" s="7"/>
-      <c r="CK20">
-        <v>1</v>
-      </c>
-      <c r="CU20" s="12">
+      <c r="BO20" s="31"/>
+      <c r="BP20" s="12">
         <v>70</v>
       </c>
-      <c r="CV20" s="1">
+      <c r="BQ20" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>64</v>
       </c>
@@ -5058,7 +4735,7 @@
       <c r="E21" s="1">
         <v>4</v>
       </c>
-      <c r="F21" s="35"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="8">
         <v>1</v>
       </c>
@@ -5074,8 +4751,8 @@
       <c r="K21" s="9">
         <v>0</v>
       </c>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
       <c r="N21" s="10">
         <v>1</v>
       </c>
@@ -5121,8 +4798,8 @@
       <c r="AB21" s="7">
         <v>0</v>
       </c>
-      <c r="AC21" s="35"/>
-      <c r="AD21" s="35"/>
+      <c r="AC21" s="31"/>
+      <c r="AD21" s="31"/>
       <c r="AE21" s="7">
         <v>1</v>
       </c>
@@ -5138,8 +4815,8 @@
       <c r="AI21" s="7">
         <v>0</v>
       </c>
-      <c r="AJ21" s="35"/>
-      <c r="AK21" s="35"/>
+      <c r="AJ21" s="31"/>
+      <c r="AK21" s="31"/>
       <c r="AL21" s="11">
         <v>0</v>
       </c>
@@ -5155,8 +4832,8 @@
       <c r="AP21" s="10">
         <v>0</v>
       </c>
-      <c r="AQ21" s="40"/>
-      <c r="AR21" s="40"/>
+      <c r="AQ21" s="36"/>
+      <c r="AR21" s="36"/>
       <c r="AS21" s="7">
         <v>0</v>
       </c>
@@ -5202,8 +4879,8 @@
       <c r="BG21" s="7">
         <v>0</v>
       </c>
-      <c r="BH21" s="35"/>
-      <c r="BI21" s="35"/>
+      <c r="BH21" s="31"/>
+      <c r="BI21" s="31"/>
       <c r="BJ21" s="7">
         <v>0</v>
       </c>
@@ -5219,19 +4896,15 @@
       <c r="BN21" s="7">
         <v>0</v>
       </c>
-      <c r="BO21" s="35"/>
-      <c r="BP21" s="7"/>
-      <c r="CL21">
-        <v>1</v>
-      </c>
-      <c r="CU21" s="12">
+      <c r="BO21" s="31"/>
+      <c r="BP21" s="12">
         <v>56</v>
       </c>
-      <c r="CV21" s="1">
+      <c r="BQ21" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>65</v>
       </c>
@@ -5247,7 +4920,7 @@
       <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="F22" s="35"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="8">
         <v>0</v>
       </c>
@@ -5263,8 +4936,8 @@
       <c r="K22" s="9">
         <v>0</v>
       </c>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
       <c r="N22" s="10">
         <v>0</v>
       </c>
@@ -5310,8 +4983,8 @@
       <c r="AB22" s="7">
         <v>0</v>
       </c>
-      <c r="AC22" s="35"/>
-      <c r="AD22" s="35"/>
+      <c r="AC22" s="31"/>
+      <c r="AD22" s="31"/>
       <c r="AE22" s="7">
         <v>0</v>
       </c>
@@ -5327,8 +5000,8 @@
       <c r="AI22" s="7">
         <v>0</v>
       </c>
-      <c r="AJ22" s="35"/>
-      <c r="AK22" s="35"/>
+      <c r="AJ22" s="31"/>
+      <c r="AK22" s="31"/>
       <c r="AL22" s="11">
         <v>0</v>
       </c>
@@ -5344,8 +5017,8 @@
       <c r="AP22" s="10">
         <v>0</v>
       </c>
-      <c r="AQ22" s="40"/>
-      <c r="AR22" s="40"/>
+      <c r="AQ22" s="36"/>
+      <c r="AR22" s="36"/>
       <c r="AS22" s="7">
         <v>0</v>
       </c>
@@ -5391,8 +5064,8 @@
       <c r="BG22" s="7">
         <v>0</v>
       </c>
-      <c r="BH22" s="35"/>
-      <c r="BI22" s="35"/>
+      <c r="BH22" s="31"/>
+      <c r="BI22" s="31"/>
       <c r="BJ22" s="7">
         <v>0</v>
       </c>
@@ -5408,19 +5081,15 @@
       <c r="BN22" s="7">
         <v>0</v>
       </c>
-      <c r="BO22" s="35"/>
-      <c r="BP22" s="7"/>
-      <c r="CK22">
-        <v>1</v>
-      </c>
-      <c r="CU22" s="12">
+      <c r="BO22" s="31"/>
+      <c r="BP22" s="12">
         <v>29</v>
       </c>
-      <c r="CV22" s="1">
+      <c r="BQ22" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>66</v>
       </c>
@@ -5436,7 +5105,7 @@
       <c r="E23" s="1">
         <v>2</v>
       </c>
-      <c r="F23" s="35"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="8">
         <v>0</v>
       </c>
@@ -5452,8 +5121,8 @@
       <c r="K23" s="9">
         <v>0</v>
       </c>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
       <c r="N23" s="10">
         <v>0</v>
       </c>
@@ -5499,8 +5168,8 @@
       <c r="AB23" s="7">
         <v>0</v>
       </c>
-      <c r="AC23" s="35"/>
-      <c r="AD23" s="35"/>
+      <c r="AC23" s="31"/>
+      <c r="AD23" s="31"/>
       <c r="AE23" s="7">
         <v>0</v>
       </c>
@@ -5516,8 +5185,8 @@
       <c r="AI23" s="7">
         <v>0</v>
       </c>
-      <c r="AJ23" s="35"/>
-      <c r="AK23" s="35"/>
+      <c r="AJ23" s="31"/>
+      <c r="AK23" s="31"/>
       <c r="AL23" s="11">
         <v>0</v>
       </c>
@@ -5533,8 +5202,8 @@
       <c r="AP23" s="10">
         <v>0</v>
       </c>
-      <c r="AQ23" s="40"/>
-      <c r="AR23" s="40"/>
+      <c r="AQ23" s="36"/>
+      <c r="AR23" s="36"/>
       <c r="AS23" s="7">
         <v>0</v>
       </c>
@@ -5580,8 +5249,8 @@
       <c r="BG23" s="7">
         <v>0</v>
       </c>
-      <c r="BH23" s="35"/>
-      <c r="BI23" s="35"/>
+      <c r="BH23" s="31"/>
+      <c r="BI23" s="31"/>
       <c r="BJ23" s="7">
         <v>0</v>
       </c>
@@ -5597,19 +5266,15 @@
       <c r="BN23" s="7">
         <v>0</v>
       </c>
-      <c r="BO23" s="35"/>
-      <c r="BP23" s="7"/>
-      <c r="CK23">
-        <v>1</v>
-      </c>
-      <c r="CU23" s="12">
+      <c r="BO23" s="31"/>
+      <c r="BP23" s="12">
         <v>29</v>
       </c>
-      <c r="CV23" s="1">
+      <c r="BQ23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>67</v>
       </c>
@@ -5625,7 +5290,7 @@
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="35"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="8">
         <v>1</v>
       </c>
@@ -5641,8 +5306,8 @@
       <c r="K24" s="9">
         <v>1</v>
       </c>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
       <c r="N24" s="10">
         <v>1</v>
       </c>
@@ -5688,8 +5353,8 @@
       <c r="AB24" s="7">
         <v>1</v>
       </c>
-      <c r="AC24" s="35"/>
-      <c r="AD24" s="35"/>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="31"/>
       <c r="AE24" s="7">
         <v>1</v>
       </c>
@@ -5705,8 +5370,8 @@
       <c r="AI24" s="7">
         <v>1</v>
       </c>
-      <c r="AJ24" s="35"/>
-      <c r="AK24" s="35"/>
+      <c r="AJ24" s="31"/>
+      <c r="AK24" s="31"/>
       <c r="AL24" s="11">
         <v>0</v>
       </c>
@@ -5722,8 +5387,8 @@
       <c r="AP24" s="10">
         <v>0</v>
       </c>
-      <c r="AQ24" s="40"/>
-      <c r="AR24" s="40"/>
+      <c r="AQ24" s="36"/>
+      <c r="AR24" s="36"/>
       <c r="AS24" s="7">
         <v>0</v>
       </c>
@@ -5769,8 +5434,8 @@
       <c r="BG24" s="7">
         <v>0</v>
       </c>
-      <c r="BH24" s="35"/>
-      <c r="BI24" s="35"/>
+      <c r="BH24" s="31"/>
+      <c r="BI24" s="31"/>
       <c r="BJ24" s="7">
         <v>0</v>
       </c>
@@ -5786,16 +5451,15 @@
       <c r="BN24" s="7">
         <v>0</v>
       </c>
-      <c r="BO24" s="35"/>
-      <c r="BP24" s="7"/>
-      <c r="CU24" s="12">
+      <c r="BO24" s="31"/>
+      <c r="BP24" s="12">
         <v>73</v>
       </c>
-      <c r="CV24" s="1">
+      <c r="BQ24" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>68</v>
       </c>
@@ -5811,7 +5475,7 @@
       <c r="E25" s="1">
         <v>2</v>
       </c>
-      <c r="F25" s="35"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="8">
         <v>1</v>
       </c>
@@ -5827,8 +5491,8 @@
       <c r="K25" s="9">
         <v>1</v>
       </c>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
       <c r="N25" s="10">
         <v>1</v>
       </c>
@@ -5874,8 +5538,8 @@
       <c r="AB25" s="7">
         <v>1</v>
       </c>
-      <c r="AC25" s="35"/>
-      <c r="AD25" s="35"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="31"/>
       <c r="AE25" s="7">
         <v>1</v>
       </c>
@@ -5891,8 +5555,8 @@
       <c r="AI25" s="7">
         <v>1</v>
       </c>
-      <c r="AJ25" s="35"/>
-      <c r="AK25" s="35"/>
+      <c r="AJ25" s="31"/>
+      <c r="AK25" s="31"/>
       <c r="AL25" s="11">
         <v>0</v>
       </c>
@@ -5908,8 +5572,8 @@
       <c r="AP25" s="10">
         <v>0</v>
       </c>
-      <c r="AQ25" s="40"/>
-      <c r="AR25" s="40"/>
+      <c r="AQ25" s="36"/>
+      <c r="AR25" s="36"/>
       <c r="AS25" s="7">
         <v>0</v>
       </c>
@@ -5955,8 +5619,8 @@
       <c r="BG25" s="7">
         <v>0</v>
       </c>
-      <c r="BH25" s="35"/>
-      <c r="BI25" s="35"/>
+      <c r="BH25" s="31"/>
+      <c r="BI25" s="31"/>
       <c r="BJ25" s="7">
         <v>0</v>
       </c>
@@ -5972,19 +5636,15 @@
       <c r="BN25" s="7">
         <v>0</v>
       </c>
-      <c r="BO25" s="35"/>
-      <c r="BP25" s="7"/>
-      <c r="CA25">
-        <v>1</v>
-      </c>
-      <c r="CU25" s="12">
+      <c r="BO25" s="31"/>
+      <c r="BP25" s="12">
         <v>73</v>
       </c>
-      <c r="CV25" s="1">
+      <c r="BQ25" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>69</v>
       </c>
@@ -6000,7 +5660,7 @@
       <c r="E26" s="1">
         <v>3</v>
       </c>
-      <c r="F26" s="35"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="8">
         <v>1</v>
       </c>
@@ -6016,8 +5676,8 @@
       <c r="K26" s="9">
         <v>0</v>
       </c>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
       <c r="N26" s="10">
         <v>1</v>
       </c>
@@ -6063,8 +5723,8 @@
       <c r="AB26" s="7">
         <v>0</v>
       </c>
-      <c r="AC26" s="35"/>
-      <c r="AD26" s="35"/>
+      <c r="AC26" s="31"/>
+      <c r="AD26" s="31"/>
       <c r="AE26" s="7">
         <v>1</v>
       </c>
@@ -6080,8 +5740,8 @@
       <c r="AI26" s="7">
         <v>0</v>
       </c>
-      <c r="AJ26" s="35"/>
-      <c r="AK26" s="35"/>
+      <c r="AJ26" s="31"/>
+      <c r="AK26" s="31"/>
       <c r="AL26" s="11">
         <v>0</v>
       </c>
@@ -6097,8 +5757,8 @@
       <c r="AP26" s="10">
         <v>0</v>
       </c>
-      <c r="AQ26" s="40"/>
-      <c r="AR26" s="40"/>
+      <c r="AQ26" s="36"/>
+      <c r="AR26" s="36"/>
       <c r="AS26" s="7">
         <v>0</v>
       </c>
@@ -6144,8 +5804,8 @@
       <c r="BG26" s="7">
         <v>0</v>
       </c>
-      <c r="BH26" s="35"/>
-      <c r="BI26" s="35"/>
+      <c r="BH26" s="31"/>
+      <c r="BI26" s="31"/>
       <c r="BJ26" s="7">
         <v>0</v>
       </c>
@@ -6161,19 +5821,15 @@
       <c r="BN26" s="7">
         <v>0</v>
       </c>
-      <c r="BO26" s="35"/>
-      <c r="BP26" s="7"/>
-      <c r="CK26">
-        <v>1</v>
-      </c>
-      <c r="CU26" s="12">
+      <c r="BO26" s="31"/>
+      <c r="BP26" s="12">
         <v>41</v>
       </c>
-      <c r="CV26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:100" x14ac:dyDescent="0.2">
+      <c r="BQ26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>70</v>
       </c>
@@ -6189,7 +5845,7 @@
       <c r="E27" s="1">
         <v>3</v>
       </c>
-      <c r="F27" s="35"/>
+      <c r="F27" s="31"/>
       <c r="G27" s="8">
         <v>0</v>
       </c>
@@ -6205,8 +5861,8 @@
       <c r="K27" s="9">
         <v>0</v>
       </c>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
       <c r="N27" s="10">
         <v>0</v>
       </c>
@@ -6252,8 +5908,8 @@
       <c r="AB27" s="7">
         <v>0</v>
       </c>
-      <c r="AC27" s="35"/>
-      <c r="AD27" s="35"/>
+      <c r="AC27" s="31"/>
+      <c r="AD27" s="31"/>
       <c r="AE27" s="7">
         <v>0</v>
       </c>
@@ -6269,8 +5925,8 @@
       <c r="AI27" s="7">
         <v>0</v>
       </c>
-      <c r="AJ27" s="35"/>
-      <c r="AK27" s="35"/>
+      <c r="AJ27" s="31"/>
+      <c r="AK27" s="31"/>
       <c r="AL27" s="11">
         <v>0</v>
       </c>
@@ -6286,8 +5942,8 @@
       <c r="AP27" s="10">
         <v>0</v>
       </c>
-      <c r="AQ27" s="40"/>
-      <c r="AR27" s="40"/>
+      <c r="AQ27" s="36"/>
+      <c r="AR27" s="36"/>
       <c r="AS27" s="7">
         <v>0</v>
       </c>
@@ -6333,8 +5989,8 @@
       <c r="BG27" s="7">
         <v>0</v>
       </c>
-      <c r="BH27" s="35"/>
-      <c r="BI27" s="35"/>
+      <c r="BH27" s="31"/>
+      <c r="BI27" s="31"/>
       <c r="BJ27" s="7">
         <v>0</v>
       </c>
@@ -6350,19 +6006,15 @@
       <c r="BN27" s="7">
         <v>0</v>
       </c>
-      <c r="BO27" s="35"/>
-      <c r="BP27" s="7"/>
-      <c r="CK27">
-        <v>1</v>
-      </c>
-      <c r="CU27" s="12">
+      <c r="BO27" s="31"/>
+      <c r="BP27" s="12">
         <v>15</v>
       </c>
-      <c r="CV27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:100" x14ac:dyDescent="0.2">
+      <c r="BQ27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>71</v>
       </c>
@@ -6378,7 +6030,7 @@
       <c r="E28" s="1">
         <v>1</v>
       </c>
-      <c r="F28" s="35"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="8">
         <v>1</v>
       </c>
@@ -6394,8 +6046,8 @@
       <c r="K28" s="9">
         <v>1</v>
       </c>
-      <c r="L28" s="35"/>
-      <c r="M28" s="35"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
       <c r="N28" s="10">
         <v>0</v>
       </c>
@@ -6441,8 +6093,8 @@
       <c r="AB28" s="7">
         <v>0</v>
       </c>
-      <c r="AC28" s="35"/>
-      <c r="AD28" s="35"/>
+      <c r="AC28" s="31"/>
+      <c r="AD28" s="31"/>
       <c r="AE28" s="7">
         <v>1</v>
       </c>
@@ -6458,8 +6110,8 @@
       <c r="AI28" s="7">
         <v>1</v>
       </c>
-      <c r="AJ28" s="35"/>
-      <c r="AK28" s="35"/>
+      <c r="AJ28" s="31"/>
+      <c r="AK28" s="31"/>
       <c r="AL28" s="11">
         <v>1</v>
       </c>
@@ -6475,8 +6127,8 @@
       <c r="AP28" s="10">
         <v>0</v>
       </c>
-      <c r="AQ28" s="40"/>
-      <c r="AR28" s="40"/>
+      <c r="AQ28" s="36"/>
+      <c r="AR28" s="36"/>
       <c r="AS28" s="7">
         <v>1</v>
       </c>
@@ -6522,8 +6174,8 @@
       <c r="BG28" s="7">
         <v>0</v>
       </c>
-      <c r="BH28" s="35"/>
-      <c r="BI28" s="35"/>
+      <c r="BH28" s="31"/>
+      <c r="BI28" s="31"/>
       <c r="BJ28" s="7">
         <v>0</v>
       </c>
@@ -6539,19 +6191,73 @@
       <c r="BN28" s="7">
         <v>0</v>
       </c>
-      <c r="BO28" s="35"/>
-      <c r="BP28" s="7"/>
-      <c r="CR28">
-        <v>1</v>
-      </c>
-      <c r="CU28" s="12">
+      <c r="BO28" s="31"/>
+      <c r="BP28" s="12">
         <v>55</v>
       </c>
-      <c r="CV28" s="1">
+      <c r="BQ28" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BQ28" xr:uid="{E0647D70-5AFF-3445-8F6E-0A0D2D26478E}">
+    <filterColumn colId="6" showButton="0"/>
+    <filterColumn colId="7" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+    <filterColumn colId="10" showButton="0"/>
+    <filterColumn colId="11" showButton="0"/>
+    <filterColumn colId="12" showButton="0"/>
+    <filterColumn colId="13" showButton="0"/>
+    <filterColumn colId="14" showButton="0"/>
+    <filterColumn colId="15" showButton="0"/>
+    <filterColumn colId="16" showButton="0"/>
+    <filterColumn colId="17" showButton="0"/>
+    <filterColumn colId="18" showButton="0"/>
+    <filterColumn colId="19" showButton="0"/>
+    <filterColumn colId="20" showButton="0"/>
+    <filterColumn colId="21" showButton="0"/>
+    <filterColumn colId="22" showButton="0"/>
+    <filterColumn colId="23" showButton="0"/>
+    <filterColumn colId="24" showButton="0"/>
+    <filterColumn colId="25" showButton="0"/>
+    <filterColumn colId="26" showButton="0"/>
+    <filterColumn colId="27" showButton="0"/>
+    <filterColumn colId="28" showButton="0"/>
+    <filterColumn colId="29" showButton="0"/>
+    <filterColumn colId="30" showButton="0"/>
+    <filterColumn colId="31" showButton="0"/>
+    <filterColumn colId="32" showButton="0"/>
+    <filterColumn colId="33" showButton="0"/>
+    <filterColumn colId="37" showButton="0"/>
+    <filterColumn colId="38" showButton="0"/>
+    <filterColumn colId="39" showButton="0"/>
+    <filterColumn colId="40" showButton="0"/>
+    <filterColumn colId="41" showButton="0"/>
+    <filterColumn colId="42" showButton="0"/>
+    <filterColumn colId="43" showButton="0"/>
+    <filterColumn colId="44" showButton="0"/>
+    <filterColumn colId="45" showButton="0"/>
+    <filterColumn colId="46" showButton="0"/>
+    <filterColumn colId="47" showButton="0"/>
+    <filterColumn colId="48" showButton="0"/>
+    <filterColumn colId="49" showButton="0"/>
+    <filterColumn colId="50" showButton="0"/>
+    <filterColumn colId="51" showButton="0"/>
+    <filterColumn colId="52" showButton="0"/>
+    <filterColumn colId="53" showButton="0"/>
+    <filterColumn colId="54" showButton="0"/>
+    <filterColumn colId="55" showButton="0"/>
+    <filterColumn colId="56" showButton="0"/>
+    <filterColumn colId="57" showButton="0"/>
+    <filterColumn colId="58" showButton="0"/>
+    <filterColumn colId="59" showButton="0"/>
+    <filterColumn colId="60" showButton="0"/>
+    <filterColumn colId="61" showButton="0"/>
+    <filterColumn colId="62" showButton="0"/>
+    <filterColumn colId="63" showButton="0"/>
+    <filterColumn colId="64" showButton="0"/>
+  </autoFilter>
   <mergeCells count="18">
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="Q3:S3"/>

</xml_diff>

<commit_message>
change land drainage change in change.xlxs to match Simon's
</commit_message>
<xml_diff>
--- a/Butterfly matrix.xlsx
+++ b/Butterfly matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FA8BCC-0DF0-6045-B43B-6759284E7FD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F830A04-5E6B-C643-B651-FBD8746C8A45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Species Set" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="164">
   <si>
     <t>Species</t>
   </si>
@@ -641,6 +641,12 @@
   </si>
   <si>
     <t>L_G3_late</t>
+  </si>
+  <si>
+    <t>L_gens_start</t>
+  </si>
+  <si>
+    <t>L_gens_end</t>
   </si>
 </sst>
 </file>
@@ -921,6 +927,36 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -940,36 +976,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1364,8 +1370,8 @@
   <dimension ref="A1:CQ28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BS28" sqref="BS28"/>
+      <pane xSplit="1" topLeftCell="AU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AV16" sqref="AV16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1417,189 +1423,189 @@
     <col min="86" max="86" width="17.6640625" customWidth="1"/>
     <col min="87" max="87" width="19.6640625" customWidth="1"/>
     <col min="89" max="94" width="10" customWidth="1"/>
-    <col min="95" max="95" width="10" style="46" customWidth="1"/>
+    <col min="95" max="95" width="10" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:95" x14ac:dyDescent="0.2">
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40"/>
-      <c r="AM1" s="40"/>
-      <c r="AN1" s="40"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="40"/>
-      <c r="AQ1" s="40"/>
-      <c r="AR1" s="40"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="52"/>
+      <c r="AD1" s="52"/>
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="52"/>
+      <c r="AK1" s="52"/>
+      <c r="AL1" s="52"/>
+      <c r="AM1" s="52"/>
+      <c r="AN1" s="52"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="52"/>
+      <c r="AQ1" s="52"/>
+      <c r="AR1" s="52"/>
       <c r="AS1" s="34"/>
       <c r="AT1" s="34"/>
-      <c r="AU1" s="41" t="s">
+      <c r="AU1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="AV1" s="41"/>
-      <c r="AW1" s="41"/>
-      <c r="AX1" s="41"/>
-      <c r="AY1" s="41"/>
-      <c r="AZ1" s="41"/>
-      <c r="BA1" s="41"/>
-      <c r="BB1" s="41"/>
-      <c r="BC1" s="41"/>
-      <c r="BD1" s="41"/>
-      <c r="BE1" s="41"/>
-      <c r="BF1" s="41"/>
-      <c r="BG1" s="41"/>
-      <c r="BH1" s="41"/>
-      <c r="BI1" s="41"/>
-      <c r="BJ1" s="41"/>
-      <c r="BK1" s="41"/>
-      <c r="BL1" s="41"/>
-      <c r="BM1" s="41"/>
-      <c r="BN1" s="41"/>
-      <c r="BO1" s="41"/>
-      <c r="BP1" s="41"/>
-      <c r="BQ1" s="41"/>
-      <c r="BR1" s="41"/>
-      <c r="BS1" s="41"/>
-      <c r="BT1" s="41"/>
-      <c r="BU1" s="41"/>
-      <c r="BV1" s="41"/>
-      <c r="BW1" s="41"/>
-      <c r="BX1" s="41"/>
-      <c r="BY1" s="41"/>
-      <c r="BZ1" s="41"/>
-      <c r="CA1" s="41"/>
-      <c r="CB1" s="41"/>
-      <c r="CC1" s="41"/>
-      <c r="CD1" s="41"/>
-      <c r="CE1" s="41"/>
-      <c r="CF1" s="41"/>
+      <c r="AV1" s="53"/>
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="53"/>
+      <c r="AZ1" s="53"/>
+      <c r="BA1" s="53"/>
+      <c r="BB1" s="53"/>
+      <c r="BC1" s="53"/>
+      <c r="BD1" s="53"/>
+      <c r="BE1" s="53"/>
+      <c r="BF1" s="53"/>
+      <c r="BG1" s="53"/>
+      <c r="BH1" s="53"/>
+      <c r="BI1" s="53"/>
+      <c r="BJ1" s="53"/>
+      <c r="BK1" s="53"/>
+      <c r="BL1" s="53"/>
+      <c r="BM1" s="53"/>
+      <c r="BN1" s="53"/>
+      <c r="BO1" s="53"/>
+      <c r="BP1" s="53"/>
+      <c r="BQ1" s="53"/>
+      <c r="BR1" s="53"/>
+      <c r="BS1" s="53"/>
+      <c r="BT1" s="53"/>
+      <c r="BU1" s="53"/>
+      <c r="BV1" s="53"/>
+      <c r="BW1" s="53"/>
+      <c r="BX1" s="53"/>
+      <c r="BY1" s="53"/>
+      <c r="BZ1" s="53"/>
+      <c r="CA1" s="53"/>
+      <c r="CB1" s="53"/>
+      <c r="CC1" s="53"/>
+      <c r="CD1" s="53"/>
+      <c r="CE1" s="53"/>
+      <c r="CF1" s="53"/>
       <c r="CG1" s="33"/>
     </row>
     <row r="2" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="N2" s="43" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="N2" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
       <c r="AC2" s="33"/>
       <c r="AD2" s="33"/>
-      <c r="AE2" s="49" t="s">
+      <c r="AE2" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="49"/>
-      <c r="AI2" s="49"/>
-      <c r="AJ2" s="49"/>
-      <c r="AK2" s="50"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="46"/>
       <c r="AL2" s="36"/>
       <c r="AM2" s="33"/>
-      <c r="AN2" s="37" t="s">
+      <c r="AN2" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="AO2" s="38"/>
-      <c r="AP2" s="38"/>
-      <c r="AQ2" s="38"/>
-      <c r="AR2" s="38"/>
+      <c r="AO2" s="50"/>
+      <c r="AP2" s="50"/>
+      <c r="AQ2" s="50"/>
+      <c r="AR2" s="50"/>
       <c r="AS2" s="34"/>
       <c r="AT2" s="34"/>
-      <c r="AU2" s="42" t="s">
+      <c r="AU2" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="AV2" s="42"/>
-      <c r="AW2" s="42"/>
-      <c r="AX2" s="42"/>
-      <c r="AY2" s="42"/>
+      <c r="AV2" s="54"/>
+      <c r="AW2" s="54"/>
+      <c r="AX2" s="54"/>
+      <c r="AY2" s="54"/>
       <c r="AZ2" s="33"/>
       <c r="BA2" s="33"/>
-      <c r="BB2" s="43" t="s">
+      <c r="BB2" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="BC2" s="43"/>
-      <c r="BD2" s="43"/>
-      <c r="BE2" s="43"/>
-      <c r="BF2" s="43"/>
-      <c r="BG2" s="43"/>
-      <c r="BH2" s="43"/>
-      <c r="BI2" s="43"/>
-      <c r="BJ2" s="43"/>
-      <c r="BK2" s="43"/>
-      <c r="BL2" s="43"/>
-      <c r="BM2" s="43"/>
-      <c r="BN2" s="43"/>
-      <c r="BO2" s="43"/>
-      <c r="BP2" s="43"/>
+      <c r="BC2" s="55"/>
+      <c r="BD2" s="55"/>
+      <c r="BE2" s="55"/>
+      <c r="BF2" s="55"/>
+      <c r="BG2" s="55"/>
+      <c r="BH2" s="55"/>
+      <c r="BI2" s="55"/>
+      <c r="BJ2" s="55"/>
+      <c r="BK2" s="55"/>
+      <c r="BL2" s="55"/>
+      <c r="BM2" s="55"/>
+      <c r="BN2" s="55"/>
+      <c r="BO2" s="55"/>
+      <c r="BP2" s="55"/>
       <c r="BQ2" s="33"/>
       <c r="BR2" s="33"/>
-      <c r="BS2" s="49" t="s">
+      <c r="BS2" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="BT2" s="49"/>
-      <c r="BU2" s="49"/>
-      <c r="BV2" s="49"/>
-      <c r="BW2" s="49"/>
-      <c r="BX2" s="49"/>
-      <c r="BY2" s="50"/>
+      <c r="BT2" s="45"/>
+      <c r="BU2" s="45"/>
+      <c r="BV2" s="45"/>
+      <c r="BW2" s="45"/>
+      <c r="BX2" s="45"/>
+      <c r="BY2" s="46"/>
       <c r="BZ2" s="36"/>
       <c r="CA2" s="33"/>
-      <c r="CB2" s="37" t="s">
+      <c r="CB2" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="CC2" s="37"/>
-      <c r="CD2" s="37"/>
-      <c r="CE2" s="37"/>
-      <c r="CF2" s="37"/>
+      <c r="CC2" s="49"/>
+      <c r="CD2" s="49"/>
+      <c r="CE2" s="49"/>
+      <c r="CF2" s="49"/>
       <c r="CG2" s="33"/>
     </row>
     <row r="3" spans="1:95" x14ac:dyDescent="0.2">
@@ -1618,46 +1624,46 @@
       <c r="K3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="44" t="s">
+      <c r="N3" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="45" t="s">
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="44" t="s">
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="45" t="s">
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="44" t="s">
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
       <c r="AC3" s="34"/>
       <c r="AD3" s="34"/>
-      <c r="AE3" s="51" t="s">
+      <c r="AE3" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="53" t="s">
+      <c r="AF3" s="42"/>
+      <c r="AG3" s="42"/>
+      <c r="AH3" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="51" t="s">
+      <c r="AI3" s="43"/>
+      <c r="AJ3" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="AK3" s="55"/>
+      <c r="AK3" s="44"/>
       <c r="AL3" s="36"/>
       <c r="AM3" s="34"/>
       <c r="AN3" s="21" t="s">
@@ -1694,46 +1700,46 @@
       </c>
       <c r="AZ3" s="34"/>
       <c r="BA3" s="34"/>
-      <c r="BB3" s="44" t="s">
+      <c r="BB3" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="BC3" s="44"/>
-      <c r="BD3" s="44"/>
-      <c r="BE3" s="45" t="s">
+      <c r="BC3" s="47"/>
+      <c r="BD3" s="47"/>
+      <c r="BE3" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="BF3" s="45"/>
-      <c r="BG3" s="45"/>
-      <c r="BH3" s="44" t="s">
+      <c r="BF3" s="48"/>
+      <c r="BG3" s="48"/>
+      <c r="BH3" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="BI3" s="44"/>
-      <c r="BJ3" s="44"/>
-      <c r="BK3" s="45" t="s">
+      <c r="BI3" s="47"/>
+      <c r="BJ3" s="47"/>
+      <c r="BK3" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="BL3" s="45"/>
-      <c r="BM3" s="45"/>
-      <c r="BN3" s="44" t="s">
+      <c r="BL3" s="48"/>
+      <c r="BM3" s="48"/>
+      <c r="BN3" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="BO3" s="44"/>
-      <c r="BP3" s="44"/>
+      <c r="BO3" s="47"/>
+      <c r="BP3" s="47"/>
       <c r="BQ3" s="34"/>
       <c r="BR3" s="34"/>
-      <c r="BS3" s="51" t="s">
+      <c r="BS3" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="BT3" s="51"/>
-      <c r="BU3" s="51"/>
-      <c r="BV3" s="53" t="s">
+      <c r="BT3" s="42"/>
+      <c r="BU3" s="42"/>
+      <c r="BV3" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="BW3" s="53"/>
-      <c r="BX3" s="51" t="s">
+      <c r="BW3" s="43"/>
+      <c r="BX3" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="BY3" s="55"/>
+      <c r="BY3" s="44"/>
       <c r="BZ3" s="36"/>
       <c r="CA3" s="34"/>
       <c r="CB3" s="21" t="s">
@@ -1752,13 +1758,13 @@
         <v>103</v>
       </c>
       <c r="CG3" s="34"/>
-      <c r="CK3" s="47"/>
-      <c r="CL3" s="47"/>
-      <c r="CM3" s="47"/>
-      <c r="CN3" s="47"/>
-      <c r="CO3" s="47"/>
-      <c r="CP3" s="47"/>
-      <c r="CQ3" s="48"/>
+      <c r="CK3" s="38"/>
+      <c r="CL3" s="38"/>
+      <c r="CM3" s="38"/>
+      <c r="CN3" s="38"/>
+      <c r="CO3" s="38"/>
+      <c r="CP3" s="38"/>
+      <c r="CQ3" s="39"/>
     </row>
     <row r="4" spans="1:95" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1851,25 +1857,25 @@
       <c r="AD4" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="AE4" s="52" t="s">
+      <c r="AE4" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="AF4" s="52" t="s">
+      <c r="AF4" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="AG4" s="52" t="s">
+      <c r="AG4" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="AH4" s="54" t="s">
+      <c r="AH4" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="AI4" s="54" t="s">
+      <c r="AI4" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="AJ4" s="52" t="s">
+      <c r="AJ4" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="AK4" s="52" t="s">
+      <c r="AK4" s="40" t="s">
         <v>152</v>
       </c>
       <c r="AL4" s="35" t="s">
@@ -1969,31 +1975,31 @@
         <v>132</v>
       </c>
       <c r="BR4" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="BS4" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="BS4" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="BT4" s="52" t="s">
+      <c r="BT4" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="BU4" s="52" t="s">
+      <c r="BU4" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="BV4" s="54" t="s">
+      <c r="BV4" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="BW4" s="54" t="s">
+      <c r="BW4" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="BX4" s="52" t="s">
+      <c r="BX4" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="BY4" s="52" t="s">
+      <c r="BY4" s="40" t="s">
         <v>161</v>
       </c>
       <c r="BZ4" s="35" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="CA4" s="35" t="s">
         <v>133</v>
@@ -7546,6 +7552,19 @@
     <filterColumn colId="82" showButton="0"/>
   </autoFilter>
   <mergeCells count="26">
+    <mergeCell ref="CB2:CF2"/>
+    <mergeCell ref="AN2:AR2"/>
+    <mergeCell ref="G1:AR1"/>
+    <mergeCell ref="AU1:CF1"/>
+    <mergeCell ref="AU2:AY2"/>
+    <mergeCell ref="BB2:BP2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="N2:AB2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="AJ3:AK3"/>
@@ -7554,24 +7573,11 @@
     <mergeCell ref="BS3:BU3"/>
     <mergeCell ref="BV3:BW3"/>
     <mergeCell ref="BX3:BY3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
     <mergeCell ref="BB3:BD3"/>
     <mergeCell ref="BE3:BG3"/>
     <mergeCell ref="BH3:BJ3"/>
     <mergeCell ref="BK3:BM3"/>
     <mergeCell ref="BN3:BP3"/>
-    <mergeCell ref="CB2:CF2"/>
-    <mergeCell ref="AN2:AR2"/>
-    <mergeCell ref="G1:AR1"/>
-    <mergeCell ref="AU1:CF1"/>
-    <mergeCell ref="AU2:AY2"/>
-    <mergeCell ref="BB2:BP2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="N2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>